<commit_message>
Actualiza la partida en la base da datos
</commit_message>
<xml_diff>
--- a/por hacer.xlsx
+++ b/por hacer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proyecto mayo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B8AB17C-E420-47BE-80B1-57E1D78C60CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67E39536-B1B5-4BE3-A078-CA11BEB58121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2736" yWindow="1440" windowWidth="18948" windowHeight="10656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,9 +68,6 @@
     <t>Estilos targetas Fotos</t>
   </si>
   <si>
-    <t>Partidas Totalres, Gandas y Perdidas</t>
-  </si>
-  <si>
     <t>Mandar info pagina principal (Juegos)</t>
   </si>
   <si>
@@ -93,6 +90,9 @@
   </si>
   <si>
     <t>Partidas con fichas restantes, tipo de juego y que guarde el tablero y el estado de la partidas</t>
+  </si>
+  <si>
+    <t>Partidas Totales, Gandas y Perdidas</t>
   </si>
 </sst>
 </file>
@@ -526,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH167"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26:I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -879,7 +879,7 @@
       <c r="A10" s="1"/>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
@@ -917,7 +917,7 @@
       <c r="A11" s="1"/>
       <c r="B11" s="6"/>
       <c r="C11" s="9" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
@@ -1031,7 +1031,7 @@
       <c r="A14" s="1"/>
       <c r="B14" s="3"/>
       <c r="C14" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
@@ -1107,7 +1107,7 @@
       <c r="A16" s="1"/>
       <c r="B16" s="7"/>
       <c r="C16" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
@@ -1145,7 +1145,7 @@
       <c r="A17" s="1"/>
       <c r="B17" s="4"/>
       <c r="C17" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
@@ -1335,7 +1335,7 @@
       <c r="A22" s="1"/>
       <c r="B22" s="4"/>
       <c r="C22" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
@@ -1373,7 +1373,7 @@
       <c r="A23" s="1"/>
       <c r="B23" s="4"/>
       <c r="C23" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
@@ -1411,7 +1411,7 @@
       <c r="A24" s="1"/>
       <c r="B24" s="4"/>
       <c r="C24" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
@@ -1449,7 +1449,7 @@
       <c r="A25" s="1"/>
       <c r="B25" s="4"/>
       <c r="C25" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
@@ -6570,6 +6570,67 @@
     </row>
   </sheetData>
   <mergeCells count="77">
+    <mergeCell ref="C18:I18"/>
+    <mergeCell ref="B12:I12"/>
+    <mergeCell ref="C13:I13"/>
+    <mergeCell ref="C15:I15"/>
+    <mergeCell ref="C16:I16"/>
+    <mergeCell ref="C17:I17"/>
+    <mergeCell ref="C5:I5"/>
+    <mergeCell ref="C14:I14"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="C3:I3"/>
+    <mergeCell ref="C4:I4"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="C7:I7"/>
+    <mergeCell ref="C8:I8"/>
+    <mergeCell ref="C9:I9"/>
+    <mergeCell ref="C11:I11"/>
+    <mergeCell ref="C10:I10"/>
+    <mergeCell ref="C20:I20"/>
+    <mergeCell ref="C21:I21"/>
+    <mergeCell ref="C22:I22"/>
+    <mergeCell ref="C23:I23"/>
+    <mergeCell ref="C24:I24"/>
+    <mergeCell ref="C25:I25"/>
+    <mergeCell ref="C26:I26"/>
+    <mergeCell ref="C27:I27"/>
+    <mergeCell ref="C28:I28"/>
+    <mergeCell ref="C29:I29"/>
+    <mergeCell ref="C30:I30"/>
+    <mergeCell ref="C31:I31"/>
+    <mergeCell ref="C32:I32"/>
+    <mergeCell ref="C33:I33"/>
+    <mergeCell ref="C34:I34"/>
+    <mergeCell ref="C35:I35"/>
+    <mergeCell ref="C36:I36"/>
+    <mergeCell ref="C37:I37"/>
+    <mergeCell ref="C38:I38"/>
+    <mergeCell ref="C39:I39"/>
+    <mergeCell ref="C40:I40"/>
+    <mergeCell ref="C41:I41"/>
+    <mergeCell ref="C42:I42"/>
+    <mergeCell ref="C43:I43"/>
+    <mergeCell ref="C44:I44"/>
+    <mergeCell ref="C45:I45"/>
+    <mergeCell ref="C46:I46"/>
+    <mergeCell ref="C47:I47"/>
+    <mergeCell ref="C48:I48"/>
+    <mergeCell ref="C55:I55"/>
+    <mergeCell ref="C57:I57"/>
+    <mergeCell ref="C58:I58"/>
+    <mergeCell ref="C49:I49"/>
+    <mergeCell ref="C50:I50"/>
+    <mergeCell ref="C51:I51"/>
+    <mergeCell ref="C52:I52"/>
+    <mergeCell ref="C53:I53"/>
+    <mergeCell ref="C77:I77"/>
+    <mergeCell ref="C78:I78"/>
+    <mergeCell ref="C69:I69"/>
+    <mergeCell ref="C70:I70"/>
+    <mergeCell ref="C71:I71"/>
+    <mergeCell ref="C72:I72"/>
+    <mergeCell ref="C73:I73"/>
     <mergeCell ref="B19:I19"/>
     <mergeCell ref="C74:I74"/>
     <mergeCell ref="C75:I75"/>
@@ -6586,67 +6647,6 @@
     <mergeCell ref="C63:I63"/>
     <mergeCell ref="C54:I54"/>
     <mergeCell ref="C56:I56"/>
-    <mergeCell ref="C77:I77"/>
-    <mergeCell ref="C78:I78"/>
-    <mergeCell ref="C69:I69"/>
-    <mergeCell ref="C70:I70"/>
-    <mergeCell ref="C71:I71"/>
-    <mergeCell ref="C72:I72"/>
-    <mergeCell ref="C73:I73"/>
-    <mergeCell ref="C57:I57"/>
-    <mergeCell ref="C58:I58"/>
-    <mergeCell ref="C49:I49"/>
-    <mergeCell ref="C50:I50"/>
-    <mergeCell ref="C51:I51"/>
-    <mergeCell ref="C52:I52"/>
-    <mergeCell ref="C53:I53"/>
-    <mergeCell ref="C45:I45"/>
-    <mergeCell ref="C46:I46"/>
-    <mergeCell ref="C47:I47"/>
-    <mergeCell ref="C48:I48"/>
-    <mergeCell ref="C55:I55"/>
-    <mergeCell ref="C40:I40"/>
-    <mergeCell ref="C41:I41"/>
-    <mergeCell ref="C42:I42"/>
-    <mergeCell ref="C43:I43"/>
-    <mergeCell ref="C44:I44"/>
-    <mergeCell ref="C35:I35"/>
-    <mergeCell ref="C36:I36"/>
-    <mergeCell ref="C37:I37"/>
-    <mergeCell ref="C38:I38"/>
-    <mergeCell ref="C39:I39"/>
-    <mergeCell ref="C30:I30"/>
-    <mergeCell ref="C31:I31"/>
-    <mergeCell ref="C32:I32"/>
-    <mergeCell ref="C33:I33"/>
-    <mergeCell ref="C34:I34"/>
-    <mergeCell ref="C25:I25"/>
-    <mergeCell ref="C26:I26"/>
-    <mergeCell ref="C27:I27"/>
-    <mergeCell ref="C28:I28"/>
-    <mergeCell ref="C29:I29"/>
-    <mergeCell ref="C20:I20"/>
-    <mergeCell ref="C21:I21"/>
-    <mergeCell ref="C22:I22"/>
-    <mergeCell ref="C23:I23"/>
-    <mergeCell ref="C24:I24"/>
-    <mergeCell ref="C5:I5"/>
-    <mergeCell ref="C14:I14"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="C3:I3"/>
-    <mergeCell ref="C4:I4"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="C7:I7"/>
-    <mergeCell ref="C8:I8"/>
-    <mergeCell ref="C9:I9"/>
-    <mergeCell ref="C11:I11"/>
-    <mergeCell ref="C10:I10"/>
-    <mergeCell ref="C18:I18"/>
-    <mergeCell ref="B12:I12"/>
-    <mergeCell ref="C13:I13"/>
-    <mergeCell ref="C15:I15"/>
-    <mergeCell ref="C16:I16"/>
-    <mergeCell ref="C17:I17"/>
   </mergeCells>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6654,6 +6654,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101001CF815299FD08446828E528E2628D888" ma:contentTypeVersion="18" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="eda16f0b0df14eff352f61fdd29391dd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f2ea13ae-bb87-41e3-80ee-445ef9952b1b" xmlns:ns4="7e6392ed-20ae-4cf8-a2eb-b9a38b6c7442" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="39a5156d44086f184d4900c1f32878c2" ns3:_="" ns4:_="">
     <xsd:import namespace="f2ea13ae-bb87-41e3-80ee-445ef9952b1b"/>
@@ -6906,15 +6915,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -6924,6 +6924,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{511756B6-1F99-4910-A3C6-88D26ECE21F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{544664A2-1060-4B74-93C6-D9FAA1CADC8A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6938,14 +6946,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{511756B6-1F99-4910-A3C6-88D26ECE21F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
mejor nombre de una variable da el id tambien, powerpoint
</commit_message>
<xml_diff>
--- a/por hacer.xlsx
+++ b/por hacer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proyecto mayo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67E39536-B1B5-4BE3-A078-CA11BEB58121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E312BC47-2CA0-42A2-BC14-670ED418EF8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2736" yWindow="1440" windowWidth="18948" windowHeight="10656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Titulo presente Pagina</t>
   </si>
@@ -80,12 +80,6 @@
     <t>Optimizar la página para que su tamaño se minimice y el código se agilice</t>
   </si>
   <si>
-    <t xml:space="preserve">Documentación de la audiencia hacia la que va dirigida la web y características de diseño </t>
-  </si>
-  <si>
-    <t>Storyboard con los efectos y animaciones que se van a utilizar</t>
-  </si>
-  <si>
     <t>Guía de estilos  que se van a utilizar.</t>
   </si>
   <si>
@@ -120,7 +114,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -145,6 +139,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -158,7 +158,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -181,7 +181,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -189,6 +189,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -524,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH167"/>
+  <dimension ref="A1:AH165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26:I26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -763,7 +766,7 @@
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="5"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="9" t="s">
         <v>2</v>
       </c>
@@ -877,9 +880,9 @@
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
-      <c r="B10" s="8"/>
+      <c r="B10" s="5"/>
       <c r="C10" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
@@ -917,7 +920,7 @@
       <c r="A11" s="1"/>
       <c r="B11" s="6"/>
       <c r="C11" s="9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
@@ -1105,7 +1108,7 @@
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
-      <c r="B16" s="7"/>
+      <c r="B16" s="4"/>
       <c r="C16" s="9" t="s">
         <v>17</v>
       </c>
@@ -1257,7 +1260,7 @@
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
-      <c r="B20" s="4"/>
+      <c r="B20" s="8"/>
       <c r="C20" s="9" t="s">
         <v>9</v>
       </c>
@@ -1295,7 +1298,7 @@
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
-      <c r="B21" s="4"/>
+      <c r="B21" s="8"/>
       <c r="C21" s="9" t="s">
         <v>10</v>
       </c>
@@ -1371,7 +1374,7 @@
     </row>
     <row r="23" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
-      <c r="B23" s="4"/>
+      <c r="B23" s="7"/>
       <c r="C23" s="9" t="s">
         <v>19</v>
       </c>
@@ -1409,10 +1412,8 @@
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="9" t="s">
-        <v>20</v>
-      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="9"/>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
@@ -1447,10 +1448,8 @@
     </row>
     <row r="25" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="9" t="s">
-        <v>21</v>
-      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="9"/>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
@@ -3322,13 +3321,13 @@
     <row r="77" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
-      <c r="C77" s="9"/>
-      <c r="D77" s="9"/>
-      <c r="E77" s="9"/>
-      <c r="F77" s="9"/>
-      <c r="G77" s="9"/>
-      <c r="H77" s="9"/>
-      <c r="I77" s="9"/>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1"/>
+      <c r="F77" s="1"/>
+      <c r="G77" s="1"/>
+      <c r="H77" s="1"/>
+      <c r="I77" s="1"/>
       <c r="J77" s="1"/>
       <c r="K77" s="1"/>
       <c r="L77" s="1"/>
@@ -3358,13 +3357,13 @@
     <row r="78" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
-      <c r="C78" s="9"/>
-      <c r="D78" s="9"/>
-      <c r="E78" s="9"/>
-      <c r="F78" s="9"/>
-      <c r="G78" s="9"/>
-      <c r="H78" s="9"/>
-      <c r="I78" s="9"/>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1"/>
+      <c r="F78" s="1"/>
+      <c r="G78" s="1"/>
+      <c r="H78" s="1"/>
+      <c r="I78" s="1"/>
       <c r="J78" s="1"/>
       <c r="K78" s="1"/>
       <c r="L78" s="1"/>
@@ -6488,8 +6487,6 @@
       <c r="AH164" s="1"/>
     </row>
     <row r="165" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A165" s="1"/>
-      <c r="B165" s="1"/>
       <c r="C165" s="1"/>
       <c r="D165" s="1"/>
       <c r="E165" s="1"/>
@@ -6497,99 +6494,29 @@
       <c r="G165" s="1"/>
       <c r="H165" s="1"/>
       <c r="I165" s="1"/>
-      <c r="J165" s="1"/>
-      <c r="K165" s="1"/>
-      <c r="L165" s="1"/>
-      <c r="M165" s="1"/>
-      <c r="N165" s="1"/>
-      <c r="O165" s="1"/>
-      <c r="P165" s="1"/>
-      <c r="Q165" s="1"/>
-      <c r="R165" s="1"/>
-      <c r="S165" s="1"/>
-      <c r="T165" s="1"/>
-      <c r="U165" s="1"/>
-      <c r="V165" s="1"/>
-      <c r="W165" s="1"/>
-      <c r="X165" s="1"/>
-      <c r="Y165" s="1"/>
-      <c r="Z165" s="1"/>
-      <c r="AA165" s="1"/>
-      <c r="AB165" s="1"/>
-      <c r="AC165" s="1"/>
-      <c r="AD165" s="1"/>
-      <c r="AE165" s="1"/>
-      <c r="AF165" s="1"/>
-      <c r="AG165" s="1"/>
-      <c r="AH165" s="1"/>
-    </row>
-    <row r="166" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A166" s="1"/>
-      <c r="B166" s="1"/>
-      <c r="C166" s="1"/>
-      <c r="D166" s="1"/>
-      <c r="E166" s="1"/>
-      <c r="F166" s="1"/>
-      <c r="G166" s="1"/>
-      <c r="H166" s="1"/>
-      <c r="I166" s="1"/>
-      <c r="J166" s="1"/>
-      <c r="K166" s="1"/>
-      <c r="L166" s="1"/>
-      <c r="M166" s="1"/>
-      <c r="N166" s="1"/>
-      <c r="O166" s="1"/>
-      <c r="P166" s="1"/>
-      <c r="Q166" s="1"/>
-      <c r="R166" s="1"/>
-      <c r="S166" s="1"/>
-      <c r="T166" s="1"/>
-      <c r="U166" s="1"/>
-      <c r="V166" s="1"/>
-      <c r="W166" s="1"/>
-      <c r="X166" s="1"/>
-      <c r="Y166" s="1"/>
-      <c r="Z166" s="1"/>
-      <c r="AA166" s="1"/>
-      <c r="AB166" s="1"/>
-      <c r="AC166" s="1"/>
-      <c r="AD166" s="1"/>
-      <c r="AE166" s="1"/>
-      <c r="AF166" s="1"/>
-      <c r="AG166" s="1"/>
-      <c r="AH166" s="1"/>
-    </row>
-    <row r="167" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="C167" s="1"/>
-      <c r="D167" s="1"/>
-      <c r="E167" s="1"/>
-      <c r="F167" s="1"/>
-      <c r="G167" s="1"/>
-      <c r="H167" s="1"/>
-      <c r="I167" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="77">
+  <mergeCells count="75">
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="C3:I3"/>
+    <mergeCell ref="C4:I4"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="C7:I7"/>
+    <mergeCell ref="C20:I20"/>
+    <mergeCell ref="C21:I21"/>
+    <mergeCell ref="C22:I22"/>
+    <mergeCell ref="C5:I5"/>
+    <mergeCell ref="C14:I14"/>
+    <mergeCell ref="C8:I8"/>
+    <mergeCell ref="C9:I9"/>
+    <mergeCell ref="C11:I11"/>
+    <mergeCell ref="C10:I10"/>
     <mergeCell ref="C18:I18"/>
     <mergeCell ref="B12:I12"/>
     <mergeCell ref="C13:I13"/>
     <mergeCell ref="C15:I15"/>
     <mergeCell ref="C16:I16"/>
     <mergeCell ref="C17:I17"/>
-    <mergeCell ref="C5:I5"/>
-    <mergeCell ref="C14:I14"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="C3:I3"/>
-    <mergeCell ref="C4:I4"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="C7:I7"/>
-    <mergeCell ref="C8:I8"/>
-    <mergeCell ref="C9:I9"/>
-    <mergeCell ref="C11:I11"/>
-    <mergeCell ref="C10:I10"/>
-    <mergeCell ref="C20:I20"/>
-    <mergeCell ref="C21:I21"/>
-    <mergeCell ref="C22:I22"/>
     <mergeCell ref="C23:I23"/>
     <mergeCell ref="C24:I24"/>
     <mergeCell ref="C25:I25"/>
@@ -6614,39 +6541,37 @@
     <mergeCell ref="C44:I44"/>
     <mergeCell ref="C45:I45"/>
     <mergeCell ref="C46:I46"/>
+    <mergeCell ref="C53:I53"/>
+    <mergeCell ref="C55:I55"/>
+    <mergeCell ref="C56:I56"/>
     <mergeCell ref="C47:I47"/>
     <mergeCell ref="C48:I48"/>
-    <mergeCell ref="C55:I55"/>
-    <mergeCell ref="C57:I57"/>
-    <mergeCell ref="C58:I58"/>
     <mergeCell ref="C49:I49"/>
     <mergeCell ref="C50:I50"/>
     <mergeCell ref="C51:I51"/>
-    <mergeCell ref="C52:I52"/>
-    <mergeCell ref="C53:I53"/>
-    <mergeCell ref="C77:I77"/>
-    <mergeCell ref="C78:I78"/>
+    <mergeCell ref="C75:I75"/>
+    <mergeCell ref="C76:I76"/>
+    <mergeCell ref="C67:I67"/>
+    <mergeCell ref="C68:I68"/>
     <mergeCell ref="C69:I69"/>
     <mergeCell ref="C70:I70"/>
     <mergeCell ref="C71:I71"/>
+    <mergeCell ref="B19:I19"/>
     <mergeCell ref="C72:I72"/>
     <mergeCell ref="C73:I73"/>
-    <mergeCell ref="B19:I19"/>
     <mergeCell ref="C74:I74"/>
-    <mergeCell ref="C75:I75"/>
-    <mergeCell ref="C76:I76"/>
+    <mergeCell ref="C62:I62"/>
+    <mergeCell ref="C63:I63"/>
     <mergeCell ref="C64:I64"/>
     <mergeCell ref="C65:I65"/>
     <mergeCell ref="C66:I66"/>
-    <mergeCell ref="C67:I67"/>
-    <mergeCell ref="C68:I68"/>
+    <mergeCell ref="C57:I57"/>
+    <mergeCell ref="C58:I58"/>
     <mergeCell ref="C59:I59"/>
     <mergeCell ref="C60:I60"/>
     <mergeCell ref="C61:I61"/>
-    <mergeCell ref="C62:I62"/>
-    <mergeCell ref="C63:I63"/>
+    <mergeCell ref="C52:I52"/>
     <mergeCell ref="C54:I54"/>
-    <mergeCell ref="C56:I56"/>
   </mergeCells>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
crear partidas filtrar por partidacambio de powerpoin y excel
</commit_message>
<xml_diff>
--- a/por hacer.xlsx
+++ b/por hacer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proyecto mayo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E312BC47-2CA0-42A2-BC14-670ED418EF8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{001784F3-8065-4D65-ABC9-5FE698C32DA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2736" yWindow="1440" windowWidth="18948" windowHeight="10656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Titulo presente Pagina</t>
   </si>
@@ -38,9 +38,6 @@
   </si>
   <si>
     <t>Conectarse a la API</t>
-  </si>
-  <si>
-    <t>Pie de Pagina</t>
   </si>
   <si>
     <t xml:space="preserve"> Si el juego está implementado, se mostrará la pantalla de inicio del juego</t>
@@ -114,7 +111,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -139,12 +136,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -158,7 +149,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -175,13 +166,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -189,9 +177,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -527,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH165"/>
+  <dimension ref="A1:AH164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -576,16 +561,16 @@
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="9" t="s">
-        <v>12</v>
+      <c r="B2" s="8" t="s">
+        <v>11</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -615,15 +600,15 @@
     <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -652,16 +637,16 @@
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="9" t="s">
-        <v>13</v>
+      <c r="B4" s="6"/>
+      <c r="C4" s="8" t="s">
+        <v>12</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
@@ -691,15 +676,15 @@
     <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="4"/>
-      <c r="C5" s="9" t="s">
-        <v>14</v>
+      <c r="C5" s="8" t="s">
+        <v>13</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -728,16 +713,16 @@
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -766,16 +751,16 @@
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="9" t="s">
+      <c r="B7" s="5"/>
+      <c r="C7" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -805,15 +790,15 @@
     <row r="8" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="5"/>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
@@ -843,15 +828,15 @@
     <row r="9" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="5"/>
-      <c r="C9" s="10" t="s">
-        <v>11</v>
+      <c r="C9" s="9" t="s">
+        <v>10</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
@@ -881,15 +866,15 @@
     <row r="10" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="5"/>
-      <c r="C10" s="9" t="s">
-        <v>20</v>
+      <c r="C10" s="8" t="s">
+        <v>19</v>
       </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
@@ -918,16 +903,16 @@
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="9" t="s">
-        <v>21</v>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8" t="s">
+        <v>20</v>
       </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
@@ -956,16 +941,16 @@
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
@@ -995,15 +980,15 @@
     <row r="13" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="3"/>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
@@ -1033,15 +1018,15 @@
     <row r="14" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="3"/>
-      <c r="C14" s="9" t="s">
-        <v>15</v>
+      <c r="C14" s="8" t="s">
+        <v>14</v>
       </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
       <c r="J14" s="2"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
@@ -1070,16 +1055,16 @@
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="9" t="s">
-        <v>6</v>
+      <c r="B15" s="3"/>
+      <c r="C15" s="8" t="s">
+        <v>16</v>
       </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -1108,16 +1093,16 @@
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="9" t="s">
-        <v>17</v>
+      <c r="B16" s="6"/>
+      <c r="C16" s="8" t="s">
+        <v>15</v>
       </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -1146,16 +1131,16 @@
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="9" t="s">
-        <v>16</v>
+      <c r="B17" s="3"/>
+      <c r="C17" s="8" t="s">
+        <v>6</v>
       </c>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
@@ -1184,16 +1169,16 @@
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="9" t="s">
+      <c r="B18" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
@@ -1222,16 +1207,16 @@
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="3"/>
+      <c r="C19" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
@@ -1260,16 +1245,16 @@
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="9" t="s">
+      <c r="B20" s="3"/>
+      <c r="C20" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
@@ -1298,16 +1283,16 @@
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="9" t="s">
-        <v>10</v>
+      <c r="B21" s="4"/>
+      <c r="C21" s="8" t="s">
+        <v>17</v>
       </c>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
@@ -1336,16 +1321,16 @@
     </row>
     <row r="22" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="9" t="s">
+      <c r="B22" s="6"/>
+      <c r="C22" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
@@ -1374,16 +1359,14 @@
     </row>
     <row r="23" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
@@ -1413,13 +1396,13 @@
     <row r="24" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
@@ -1449,13 +1432,13 @@
     <row r="25" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
@@ -1485,13 +1468,13 @@
     <row r="26" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
@@ -1521,13 +1504,13 @@
     <row r="27" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
@@ -1557,13 +1540,13 @@
     <row r="28" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="9"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
@@ -1593,13 +1576,13 @@
     <row r="29" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
@@ -1629,13 +1612,13 @@
     <row r="30" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="9"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
@@ -1665,13 +1648,13 @@
     <row r="31" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
@@ -1701,13 +1684,13 @@
     <row r="32" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="9"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
@@ -1737,13 +1720,13 @@
     <row r="33" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
@@ -1773,13 +1756,13 @@
     <row r="34" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="9"/>
-      <c r="I34" s="9"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
@@ -1809,13 +1792,13 @@
     <row r="35" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="9"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
@@ -1845,13 +1828,13 @@
     <row r="36" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="9"/>
-      <c r="H36" s="9"/>
-      <c r="I36" s="9"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
@@ -1881,13 +1864,13 @@
     <row r="37" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
-      <c r="I37" s="9"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
@@ -1917,13 +1900,13 @@
     <row r="38" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9"/>
-      <c r="I38" s="9"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
@@ -1953,13 +1936,13 @@
     <row r="39" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
-      <c r="I39" s="9"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
@@ -1989,13 +1972,13 @@
     <row r="40" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="9"/>
-      <c r="G40" s="9"/>
-      <c r="H40" s="9"/>
-      <c r="I40" s="9"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="8"/>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
@@ -2025,13 +2008,13 @@
     <row r="41" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="9"/>
-      <c r="H41" s="9"/>
-      <c r="I41" s="9"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8"/>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
@@ -2061,13 +2044,13 @@
     <row r="42" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="9"/>
-      <c r="H42" s="9"/>
-      <c r="I42" s="9"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
@@ -2097,13 +2080,13 @@
     <row r="43" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
-      <c r="C43" s="9"/>
-      <c r="D43" s="9"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="9"/>
-      <c r="G43" s="9"/>
-      <c r="H43" s="9"/>
-      <c r="I43" s="9"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
@@ -2133,13 +2116,13 @@
     <row r="44" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9"/>
-      <c r="F44" s="9"/>
-      <c r="G44" s="9"/>
-      <c r="H44" s="9"/>
-      <c r="I44" s="9"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="8"/>
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
@@ -2169,13 +2152,13 @@
     <row r="45" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
-      <c r="C45" s="9"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="9"/>
-      <c r="G45" s="9"/>
-      <c r="H45" s="9"/>
-      <c r="I45" s="9"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8"/>
+      <c r="I45" s="8"/>
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
@@ -2205,13 +2188,13 @@
     <row r="46" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="9"/>
-      <c r="H46" s="9"/>
-      <c r="I46" s="9"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8"/>
+      <c r="I46" s="8"/>
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
@@ -2241,13 +2224,13 @@
     <row r="47" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
-      <c r="C47" s="9"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="9"/>
-      <c r="F47" s="9"/>
-      <c r="G47" s="9"/>
-      <c r="H47" s="9"/>
-      <c r="I47" s="9"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="8"/>
+      <c r="I47" s="8"/>
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
@@ -2277,13 +2260,13 @@
     <row r="48" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="9"/>
-      <c r="F48" s="9"/>
-      <c r="G48" s="9"/>
-      <c r="H48" s="9"/>
-      <c r="I48" s="9"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="8"/>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8"/>
+      <c r="H48" s="8"/>
+      <c r="I48" s="8"/>
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
@@ -2313,13 +2296,13 @@
     <row r="49" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
-      <c r="C49" s="9"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="9"/>
-      <c r="F49" s="9"/>
-      <c r="G49" s="9"/>
-      <c r="H49" s="9"/>
-      <c r="I49" s="9"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="8"/>
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
@@ -2349,13 +2332,13 @@
     <row r="50" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
-      <c r="C50" s="9"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="9"/>
-      <c r="G50" s="9"/>
-      <c r="H50" s="9"/>
-      <c r="I50" s="9"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="8"/>
+      <c r="G50" s="8"/>
+      <c r="H50" s="8"/>
+      <c r="I50" s="8"/>
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
       <c r="L50" s="1"/>
@@ -2385,13 +2368,13 @@
     <row r="51" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
-      <c r="C51" s="9"/>
-      <c r="D51" s="9"/>
-      <c r="E51" s="9"/>
-      <c r="F51" s="9"/>
-      <c r="G51" s="9"/>
-      <c r="H51" s="9"/>
-      <c r="I51" s="9"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="8"/>
+      <c r="F51" s="8"/>
+      <c r="G51" s="8"/>
+      <c r="H51" s="8"/>
+      <c r="I51" s="8"/>
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
       <c r="L51" s="1"/>
@@ -2421,13 +2404,13 @@
     <row r="52" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
-      <c r="C52" s="9"/>
-      <c r="D52" s="9"/>
-      <c r="E52" s="9"/>
-      <c r="F52" s="9"/>
-      <c r="G52" s="9"/>
-      <c r="H52" s="9"/>
-      <c r="I52" s="9"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="8"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="8"/>
+      <c r="H52" s="8"/>
+      <c r="I52" s="8"/>
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
       <c r="L52" s="1"/>
@@ -2457,13 +2440,13 @@
     <row r="53" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
-      <c r="C53" s="9"/>
-      <c r="D53" s="9"/>
-      <c r="E53" s="9"/>
-      <c r="F53" s="9"/>
-      <c r="G53" s="9"/>
-      <c r="H53" s="9"/>
-      <c r="I53" s="9"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="8"/>
+      <c r="E53" s="8"/>
+      <c r="F53" s="8"/>
+      <c r="G53" s="8"/>
+      <c r="H53" s="8"/>
+      <c r="I53" s="8"/>
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
       <c r="L53" s="1"/>
@@ -2493,13 +2476,13 @@
     <row r="54" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
-      <c r="C54" s="9"/>
-      <c r="D54" s="9"/>
-      <c r="E54" s="9"/>
-      <c r="F54" s="9"/>
-      <c r="G54" s="9"/>
-      <c r="H54" s="9"/>
-      <c r="I54" s="9"/>
+      <c r="C54" s="8"/>
+      <c r="D54" s="8"/>
+      <c r="E54" s="8"/>
+      <c r="F54" s="8"/>
+      <c r="G54" s="8"/>
+      <c r="H54" s="8"/>
+      <c r="I54" s="8"/>
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
       <c r="L54" s="1"/>
@@ -2529,13 +2512,13 @@
     <row r="55" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
-      <c r="C55" s="9"/>
-      <c r="D55" s="9"/>
-      <c r="E55" s="9"/>
-      <c r="F55" s="9"/>
-      <c r="G55" s="9"/>
-      <c r="H55" s="9"/>
-      <c r="I55" s="9"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="8"/>
+      <c r="E55" s="8"/>
+      <c r="F55" s="8"/>
+      <c r="G55" s="8"/>
+      <c r="H55" s="8"/>
+      <c r="I55" s="8"/>
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
       <c r="L55" s="1"/>
@@ -2565,13 +2548,13 @@
     <row r="56" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
-      <c r="C56" s="9"/>
-      <c r="D56" s="9"/>
-      <c r="E56" s="9"/>
-      <c r="F56" s="9"/>
-      <c r="G56" s="9"/>
-      <c r="H56" s="9"/>
-      <c r="I56" s="9"/>
+      <c r="C56" s="8"/>
+      <c r="D56" s="8"/>
+      <c r="E56" s="8"/>
+      <c r="F56" s="8"/>
+      <c r="G56" s="8"/>
+      <c r="H56" s="8"/>
+      <c r="I56" s="8"/>
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
       <c r="L56" s="1"/>
@@ -2601,13 +2584,13 @@
     <row r="57" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
-      <c r="C57" s="9"/>
-      <c r="D57" s="9"/>
-      <c r="E57" s="9"/>
-      <c r="F57" s="9"/>
-      <c r="G57" s="9"/>
-      <c r="H57" s="9"/>
-      <c r="I57" s="9"/>
+      <c r="C57" s="8"/>
+      <c r="D57" s="8"/>
+      <c r="E57" s="8"/>
+      <c r="F57" s="8"/>
+      <c r="G57" s="8"/>
+      <c r="H57" s="8"/>
+      <c r="I57" s="8"/>
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
       <c r="L57" s="1"/>
@@ -2637,13 +2620,13 @@
     <row r="58" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
-      <c r="C58" s="9"/>
-      <c r="D58" s="9"/>
-      <c r="E58" s="9"/>
-      <c r="F58" s="9"/>
-      <c r="G58" s="9"/>
-      <c r="H58" s="9"/>
-      <c r="I58" s="9"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="8"/>
+      <c r="E58" s="8"/>
+      <c r="F58" s="8"/>
+      <c r="G58" s="8"/>
+      <c r="H58" s="8"/>
+      <c r="I58" s="8"/>
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
       <c r="L58" s="1"/>
@@ -2673,13 +2656,13 @@
     <row r="59" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
-      <c r="C59" s="9"/>
-      <c r="D59" s="9"/>
-      <c r="E59" s="9"/>
-      <c r="F59" s="9"/>
-      <c r="G59" s="9"/>
-      <c r="H59" s="9"/>
-      <c r="I59" s="9"/>
+      <c r="C59" s="8"/>
+      <c r="D59" s="8"/>
+      <c r="E59" s="8"/>
+      <c r="F59" s="8"/>
+      <c r="G59" s="8"/>
+      <c r="H59" s="8"/>
+      <c r="I59" s="8"/>
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
       <c r="L59" s="1"/>
@@ -2709,13 +2692,13 @@
     <row r="60" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
-      <c r="C60" s="9"/>
-      <c r="D60" s="9"/>
-      <c r="E60" s="9"/>
-      <c r="F60" s="9"/>
-      <c r="G60" s="9"/>
-      <c r="H60" s="9"/>
-      <c r="I60" s="9"/>
+      <c r="C60" s="8"/>
+      <c r="D60" s="8"/>
+      <c r="E60" s="8"/>
+      <c r="F60" s="8"/>
+      <c r="G60" s="8"/>
+      <c r="H60" s="8"/>
+      <c r="I60" s="8"/>
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
       <c r="L60" s="1"/>
@@ -2745,13 +2728,13 @@
     <row r="61" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
-      <c r="C61" s="9"/>
-      <c r="D61" s="9"/>
-      <c r="E61" s="9"/>
-      <c r="F61" s="9"/>
-      <c r="G61" s="9"/>
-      <c r="H61" s="9"/>
-      <c r="I61" s="9"/>
+      <c r="C61" s="8"/>
+      <c r="D61" s="8"/>
+      <c r="E61" s="8"/>
+      <c r="F61" s="8"/>
+      <c r="G61" s="8"/>
+      <c r="H61" s="8"/>
+      <c r="I61" s="8"/>
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
       <c r="L61" s="1"/>
@@ -2781,13 +2764,13 @@
     <row r="62" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
-      <c r="C62" s="9"/>
-      <c r="D62" s="9"/>
-      <c r="E62" s="9"/>
-      <c r="F62" s="9"/>
-      <c r="G62" s="9"/>
-      <c r="H62" s="9"/>
-      <c r="I62" s="9"/>
+      <c r="C62" s="8"/>
+      <c r="D62" s="8"/>
+      <c r="E62" s="8"/>
+      <c r="F62" s="8"/>
+      <c r="G62" s="8"/>
+      <c r="H62" s="8"/>
+      <c r="I62" s="8"/>
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
       <c r="L62" s="1"/>
@@ -2817,13 +2800,13 @@
     <row r="63" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
-      <c r="C63" s="9"/>
-      <c r="D63" s="9"/>
-      <c r="E63" s="9"/>
-      <c r="F63" s="9"/>
-      <c r="G63" s="9"/>
-      <c r="H63" s="9"/>
-      <c r="I63" s="9"/>
+      <c r="C63" s="8"/>
+      <c r="D63" s="8"/>
+      <c r="E63" s="8"/>
+      <c r="F63" s="8"/>
+      <c r="G63" s="8"/>
+      <c r="H63" s="8"/>
+      <c r="I63" s="8"/>
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
       <c r="L63" s="1"/>
@@ -2853,13 +2836,13 @@
     <row r="64" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
-      <c r="C64" s="9"/>
-      <c r="D64" s="9"/>
-      <c r="E64" s="9"/>
-      <c r="F64" s="9"/>
-      <c r="G64" s="9"/>
-      <c r="H64" s="9"/>
-      <c r="I64" s="9"/>
+      <c r="C64" s="8"/>
+      <c r="D64" s="8"/>
+      <c r="E64" s="8"/>
+      <c r="F64" s="8"/>
+      <c r="G64" s="8"/>
+      <c r="H64" s="8"/>
+      <c r="I64" s="8"/>
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
       <c r="L64" s="1"/>
@@ -2889,13 +2872,13 @@
     <row r="65" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
-      <c r="C65" s="9"/>
-      <c r="D65" s="9"/>
-      <c r="E65" s="9"/>
-      <c r="F65" s="9"/>
-      <c r="G65" s="9"/>
-      <c r="H65" s="9"/>
-      <c r="I65" s="9"/>
+      <c r="C65" s="8"/>
+      <c r="D65" s="8"/>
+      <c r="E65" s="8"/>
+      <c r="F65" s="8"/>
+      <c r="G65" s="8"/>
+      <c r="H65" s="8"/>
+      <c r="I65" s="8"/>
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
       <c r="L65" s="1"/>
@@ -2925,13 +2908,13 @@
     <row r="66" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
-      <c r="C66" s="9"/>
-      <c r="D66" s="9"/>
-      <c r="E66" s="9"/>
-      <c r="F66" s="9"/>
-      <c r="G66" s="9"/>
-      <c r="H66" s="9"/>
-      <c r="I66" s="9"/>
+      <c r="C66" s="8"/>
+      <c r="D66" s="8"/>
+      <c r="E66" s="8"/>
+      <c r="F66" s="8"/>
+      <c r="G66" s="8"/>
+      <c r="H66" s="8"/>
+      <c r="I66" s="8"/>
       <c r="J66" s="1"/>
       <c r="K66" s="1"/>
       <c r="L66" s="1"/>
@@ -2961,13 +2944,13 @@
     <row r="67" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
-      <c r="C67" s="9"/>
-      <c r="D67" s="9"/>
-      <c r="E67" s="9"/>
-      <c r="F67" s="9"/>
-      <c r="G67" s="9"/>
-      <c r="H67" s="9"/>
-      <c r="I67" s="9"/>
+      <c r="C67" s="8"/>
+      <c r="D67" s="8"/>
+      <c r="E67" s="8"/>
+      <c r="F67" s="8"/>
+      <c r="G67" s="8"/>
+      <c r="H67" s="8"/>
+      <c r="I67" s="8"/>
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>
@@ -2997,13 +2980,13 @@
     <row r="68" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
-      <c r="C68" s="9"/>
-      <c r="D68" s="9"/>
-      <c r="E68" s="9"/>
-      <c r="F68" s="9"/>
-      <c r="G68" s="9"/>
-      <c r="H68" s="9"/>
-      <c r="I68" s="9"/>
+      <c r="C68" s="8"/>
+      <c r="D68" s="8"/>
+      <c r="E68" s="8"/>
+      <c r="F68" s="8"/>
+      <c r="G68" s="8"/>
+      <c r="H68" s="8"/>
+      <c r="I68" s="8"/>
       <c r="J68" s="1"/>
       <c r="K68" s="1"/>
       <c r="L68" s="1"/>
@@ -3033,13 +3016,13 @@
     <row r="69" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
-      <c r="C69" s="9"/>
-      <c r="D69" s="9"/>
-      <c r="E69" s="9"/>
-      <c r="F69" s="9"/>
-      <c r="G69" s="9"/>
-      <c r="H69" s="9"/>
-      <c r="I69" s="9"/>
+      <c r="C69" s="8"/>
+      <c r="D69" s="8"/>
+      <c r="E69" s="8"/>
+      <c r="F69" s="8"/>
+      <c r="G69" s="8"/>
+      <c r="H69" s="8"/>
+      <c r="I69" s="8"/>
       <c r="J69" s="1"/>
       <c r="K69" s="1"/>
       <c r="L69" s="1"/>
@@ -3069,13 +3052,13 @@
     <row r="70" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
-      <c r="C70" s="9"/>
-      <c r="D70" s="9"/>
-      <c r="E70" s="9"/>
-      <c r="F70" s="9"/>
-      <c r="G70" s="9"/>
-      <c r="H70" s="9"/>
-      <c r="I70" s="9"/>
+      <c r="C70" s="8"/>
+      <c r="D70" s="8"/>
+      <c r="E70" s="8"/>
+      <c r="F70" s="8"/>
+      <c r="G70" s="8"/>
+      <c r="H70" s="8"/>
+      <c r="I70" s="8"/>
       <c r="J70" s="1"/>
       <c r="K70" s="1"/>
       <c r="L70" s="1"/>
@@ -3105,13 +3088,13 @@
     <row r="71" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
-      <c r="C71" s="9"/>
-      <c r="D71" s="9"/>
-      <c r="E71" s="9"/>
-      <c r="F71" s="9"/>
-      <c r="G71" s="9"/>
-      <c r="H71" s="9"/>
-      <c r="I71" s="9"/>
+      <c r="C71" s="8"/>
+      <c r="D71" s="8"/>
+      <c r="E71" s="8"/>
+      <c r="F71" s="8"/>
+      <c r="G71" s="8"/>
+      <c r="H71" s="8"/>
+      <c r="I71" s="8"/>
       <c r="J71" s="1"/>
       <c r="K71" s="1"/>
       <c r="L71" s="1"/>
@@ -3141,13 +3124,13 @@
     <row r="72" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
-      <c r="C72" s="9"/>
-      <c r="D72" s="9"/>
-      <c r="E72" s="9"/>
-      <c r="F72" s="9"/>
-      <c r="G72" s="9"/>
-      <c r="H72" s="9"/>
-      <c r="I72" s="9"/>
+      <c r="C72" s="8"/>
+      <c r="D72" s="8"/>
+      <c r="E72" s="8"/>
+      <c r="F72" s="8"/>
+      <c r="G72" s="8"/>
+      <c r="H72" s="8"/>
+      <c r="I72" s="8"/>
       <c r="J72" s="1"/>
       <c r="K72" s="1"/>
       <c r="L72" s="1"/>
@@ -3177,13 +3160,13 @@
     <row r="73" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
-      <c r="C73" s="9"/>
-      <c r="D73" s="9"/>
-      <c r="E73" s="9"/>
-      <c r="F73" s="9"/>
-      <c r="G73" s="9"/>
-      <c r="H73" s="9"/>
-      <c r="I73" s="9"/>
+      <c r="C73" s="8"/>
+      <c r="D73" s="8"/>
+      <c r="E73" s="8"/>
+      <c r="F73" s="8"/>
+      <c r="G73" s="8"/>
+      <c r="H73" s="8"/>
+      <c r="I73" s="8"/>
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
       <c r="L73" s="1"/>
@@ -3213,13 +3196,13 @@
     <row r="74" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
-      <c r="C74" s="9"/>
-      <c r="D74" s="9"/>
-      <c r="E74" s="9"/>
-      <c r="F74" s="9"/>
-      <c r="G74" s="9"/>
-      <c r="H74" s="9"/>
-      <c r="I74" s="9"/>
+      <c r="C74" s="8"/>
+      <c r="D74" s="8"/>
+      <c r="E74" s="8"/>
+      <c r="F74" s="8"/>
+      <c r="G74" s="8"/>
+      <c r="H74" s="8"/>
+      <c r="I74" s="8"/>
       <c r="J74" s="1"/>
       <c r="K74" s="1"/>
       <c r="L74" s="1"/>
@@ -3249,13 +3232,13 @@
     <row r="75" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
-      <c r="C75" s="9"/>
-      <c r="D75" s="9"/>
-      <c r="E75" s="9"/>
-      <c r="F75" s="9"/>
-      <c r="G75" s="9"/>
-      <c r="H75" s="9"/>
-      <c r="I75" s="9"/>
+      <c r="C75" s="8"/>
+      <c r="D75" s="8"/>
+      <c r="E75" s="8"/>
+      <c r="F75" s="8"/>
+      <c r="G75" s="8"/>
+      <c r="H75" s="8"/>
+      <c r="I75" s="8"/>
       <c r="J75" s="1"/>
       <c r="K75" s="1"/>
       <c r="L75" s="1"/>
@@ -3285,13 +3268,13 @@
     <row r="76" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
-      <c r="C76" s="9"/>
-      <c r="D76" s="9"/>
-      <c r="E76" s="9"/>
-      <c r="F76" s="9"/>
-      <c r="G76" s="9"/>
-      <c r="H76" s="9"/>
-      <c r="I76" s="9"/>
+      <c r="C76" s="1"/>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1"/>
+      <c r="F76" s="1"/>
+      <c r="G76" s="1"/>
+      <c r="H76" s="1"/>
+      <c r="I76" s="1"/>
       <c r="J76" s="1"/>
       <c r="K76" s="1"/>
       <c r="L76" s="1"/>
@@ -6451,8 +6434,6 @@
       <c r="AH163" s="1"/>
     </row>
     <row r="164" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A164" s="1"/>
-      <c r="B164" s="1"/>
       <c r="C164" s="1"/>
       <c r="D164" s="1"/>
       <c r="E164" s="1"/>
@@ -6460,118 +6441,83 @@
       <c r="G164" s="1"/>
       <c r="H164" s="1"/>
       <c r="I164" s="1"/>
-      <c r="J164" s="1"/>
-      <c r="K164" s="1"/>
-      <c r="L164" s="1"/>
-      <c r="M164" s="1"/>
-      <c r="N164" s="1"/>
-      <c r="O164" s="1"/>
-      <c r="P164" s="1"/>
-      <c r="Q164" s="1"/>
-      <c r="R164" s="1"/>
-      <c r="S164" s="1"/>
-      <c r="T164" s="1"/>
-      <c r="U164" s="1"/>
-      <c r="V164" s="1"/>
-      <c r="W164" s="1"/>
-      <c r="X164" s="1"/>
-      <c r="Y164" s="1"/>
-      <c r="Z164" s="1"/>
-      <c r="AA164" s="1"/>
-      <c r="AB164" s="1"/>
-      <c r="AC164" s="1"/>
-      <c r="AD164" s="1"/>
-      <c r="AE164" s="1"/>
-      <c r="AF164" s="1"/>
-      <c r="AG164" s="1"/>
-      <c r="AH164" s="1"/>
-    </row>
-    <row r="165" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="C165" s="1"/>
-      <c r="D165" s="1"/>
-      <c r="E165" s="1"/>
-      <c r="F165" s="1"/>
-      <c r="G165" s="1"/>
-      <c r="H165" s="1"/>
-      <c r="I165" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="75">
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="C3:I3"/>
-    <mergeCell ref="C4:I4"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="C7:I7"/>
+  <mergeCells count="74">
+    <mergeCell ref="C56:I56"/>
+    <mergeCell ref="C57:I57"/>
+    <mergeCell ref="C58:I58"/>
+    <mergeCell ref="C59:I59"/>
+    <mergeCell ref="C60:I60"/>
+    <mergeCell ref="C61:I61"/>
+    <mergeCell ref="C62:I62"/>
+    <mergeCell ref="C63:I63"/>
+    <mergeCell ref="C64:I64"/>
+    <mergeCell ref="C65:I65"/>
+    <mergeCell ref="C74:I74"/>
+    <mergeCell ref="C75:I75"/>
+    <mergeCell ref="C66:I66"/>
+    <mergeCell ref="C67:I67"/>
+    <mergeCell ref="C68:I68"/>
+    <mergeCell ref="C69:I69"/>
+    <mergeCell ref="C70:I70"/>
+    <mergeCell ref="C71:I71"/>
+    <mergeCell ref="C72:I72"/>
+    <mergeCell ref="C73:I73"/>
+    <mergeCell ref="C54:I54"/>
+    <mergeCell ref="C55:I55"/>
+    <mergeCell ref="C46:I46"/>
+    <mergeCell ref="C47:I47"/>
+    <mergeCell ref="C48:I48"/>
+    <mergeCell ref="C49:I49"/>
+    <mergeCell ref="C50:I50"/>
+    <mergeCell ref="C51:I51"/>
+    <mergeCell ref="C53:I53"/>
+    <mergeCell ref="C42:I42"/>
+    <mergeCell ref="C43:I43"/>
+    <mergeCell ref="C44:I44"/>
+    <mergeCell ref="C45:I45"/>
+    <mergeCell ref="C52:I52"/>
+    <mergeCell ref="C37:I37"/>
+    <mergeCell ref="C38:I38"/>
+    <mergeCell ref="C39:I39"/>
+    <mergeCell ref="C40:I40"/>
+    <mergeCell ref="C41:I41"/>
+    <mergeCell ref="C32:I32"/>
+    <mergeCell ref="C33:I33"/>
+    <mergeCell ref="C34:I34"/>
+    <mergeCell ref="C35:I35"/>
+    <mergeCell ref="C36:I36"/>
+    <mergeCell ref="C27:I27"/>
+    <mergeCell ref="C28:I28"/>
+    <mergeCell ref="C29:I29"/>
+    <mergeCell ref="C30:I30"/>
+    <mergeCell ref="C31:I31"/>
+    <mergeCell ref="C22:I22"/>
+    <mergeCell ref="C23:I23"/>
+    <mergeCell ref="C24:I24"/>
+    <mergeCell ref="C25:I25"/>
+    <mergeCell ref="C26:I26"/>
+    <mergeCell ref="C19:I19"/>
     <mergeCell ref="C20:I20"/>
     <mergeCell ref="C21:I21"/>
-    <mergeCell ref="C22:I22"/>
     <mergeCell ref="C5:I5"/>
     <mergeCell ref="C14:I14"/>
     <mergeCell ref="C8:I8"/>
     <mergeCell ref="C9:I9"/>
     <mergeCell ref="C11:I11"/>
     <mergeCell ref="C10:I10"/>
-    <mergeCell ref="C18:I18"/>
+    <mergeCell ref="C17:I17"/>
     <mergeCell ref="B12:I12"/>
     <mergeCell ref="C13:I13"/>
     <mergeCell ref="C15:I15"/>
     <mergeCell ref="C16:I16"/>
-    <mergeCell ref="C17:I17"/>
-    <mergeCell ref="C23:I23"/>
-    <mergeCell ref="C24:I24"/>
-    <mergeCell ref="C25:I25"/>
-    <mergeCell ref="C26:I26"/>
-    <mergeCell ref="C27:I27"/>
-    <mergeCell ref="C28:I28"/>
-    <mergeCell ref="C29:I29"/>
-    <mergeCell ref="C30:I30"/>
-    <mergeCell ref="C31:I31"/>
-    <mergeCell ref="C32:I32"/>
-    <mergeCell ref="C33:I33"/>
-    <mergeCell ref="C34:I34"/>
-    <mergeCell ref="C35:I35"/>
-    <mergeCell ref="C36:I36"/>
-    <mergeCell ref="C37:I37"/>
-    <mergeCell ref="C38:I38"/>
-    <mergeCell ref="C39:I39"/>
-    <mergeCell ref="C40:I40"/>
-    <mergeCell ref="C41:I41"/>
-    <mergeCell ref="C42:I42"/>
-    <mergeCell ref="C43:I43"/>
-    <mergeCell ref="C44:I44"/>
-    <mergeCell ref="C45:I45"/>
-    <mergeCell ref="C46:I46"/>
-    <mergeCell ref="C53:I53"/>
-    <mergeCell ref="C55:I55"/>
-    <mergeCell ref="C56:I56"/>
-    <mergeCell ref="C47:I47"/>
-    <mergeCell ref="C48:I48"/>
-    <mergeCell ref="C49:I49"/>
-    <mergeCell ref="C50:I50"/>
-    <mergeCell ref="C51:I51"/>
-    <mergeCell ref="C75:I75"/>
-    <mergeCell ref="C76:I76"/>
-    <mergeCell ref="C67:I67"/>
-    <mergeCell ref="C68:I68"/>
-    <mergeCell ref="C69:I69"/>
-    <mergeCell ref="C70:I70"/>
-    <mergeCell ref="C71:I71"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="C72:I72"/>
-    <mergeCell ref="C73:I73"/>
-    <mergeCell ref="C74:I74"/>
-    <mergeCell ref="C62:I62"/>
-    <mergeCell ref="C63:I63"/>
-    <mergeCell ref="C64:I64"/>
-    <mergeCell ref="C65:I65"/>
-    <mergeCell ref="C66:I66"/>
-    <mergeCell ref="C57:I57"/>
-    <mergeCell ref="C58:I58"/>
-    <mergeCell ref="C59:I59"/>
-    <mergeCell ref="C60:I60"/>
-    <mergeCell ref="C61:I61"/>
-    <mergeCell ref="C52:I52"/>
-    <mergeCell ref="C54:I54"/>
+    <mergeCell ref="B18:I18"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="C3:I3"/>
+    <mergeCell ref="C4:I4"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="C7:I7"/>
   </mergeCells>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6579,15 +6525,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101001CF815299FD08446828E528E2628D888" ma:contentTypeVersion="18" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="eda16f0b0df14eff352f61fdd29391dd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f2ea13ae-bb87-41e3-80ee-445ef9952b1b" xmlns:ns4="7e6392ed-20ae-4cf8-a2eb-b9a38b6c7442" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="39a5156d44086f184d4900c1f32878c2" ns3:_="" ns4:_="">
     <xsd:import namespace="f2ea13ae-bb87-41e3-80ee-445ef9952b1b"/>
@@ -6840,6 +6777,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -6849,14 +6795,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{511756B6-1F99-4910-A3C6-88D26ECE21F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{544664A2-1060-4B74-93C6-D9FAA1CADC8A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6871,6 +6809,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{511756B6-1F99-4910-A3C6-88D26ECE21F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
estilos powerpoint y excel modificados
</commit_message>
<xml_diff>
--- a/por hacer.xlsx
+++ b/por hacer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proyecto mayo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{001784F3-8065-4D65-ABC9-5FE698C32DA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F00CC3-3FE1-4F7E-9A83-10500266034B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2736" yWindow="1440" windowWidth="18948" windowHeight="10656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -111,7 +111,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -121,12 +121,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -149,7 +143,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -160,16 +154,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -515,7 +503,7 @@
   <dimension ref="A1:AH164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -561,16 +549,16 @@
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -599,16 +587,16 @@
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="8" t="s">
+      <c r="B3" s="5"/>
+      <c r="C3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -637,16 +625,16 @@
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="8" t="s">
+      <c r="B4" s="5"/>
+      <c r="C4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
@@ -675,16 +663,16 @@
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="8" t="s">
+      <c r="B5" s="5"/>
+      <c r="C5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -713,16 +701,16 @@
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -751,16 +739,16 @@
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="8" t="s">
+      <c r="B7" s="4"/>
+      <c r="C7" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -789,16 +777,16 @@
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="8" t="s">
+      <c r="B8" s="4"/>
+      <c r="C8" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
@@ -827,16 +815,16 @@
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="9" t="s">
+      <c r="B9" s="4"/>
+      <c r="C9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
@@ -865,16 +853,16 @@
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="8" t="s">
+      <c r="B10" s="4"/>
+      <c r="C10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
@@ -903,16 +891,16 @@
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8" t="s">
+      <c r="B11" s="4"/>
+      <c r="C11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
@@ -941,16 +929,16 @@
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
@@ -980,15 +968,15 @@
     <row r="13" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="3"/>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
@@ -1018,15 +1006,15 @@
     <row r="14" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="3"/>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
       <c r="J14" s="2"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
@@ -1056,15 +1044,15 @@
     <row r="15" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="3"/>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -1093,16 +1081,16 @@
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="8" t="s">
+      <c r="B16" s="5"/>
+      <c r="C16" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -1132,15 +1120,15 @@
     <row r="17" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="3"/>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
@@ -1169,16 +1157,16 @@
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
@@ -1208,15 +1196,15 @@
     <row r="19" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="3"/>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
@@ -1246,15 +1234,15 @@
     <row r="20" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="3"/>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
@@ -1283,16 +1271,16 @@
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="8" t="s">
+      <c r="B21" s="3"/>
+      <c r="C21" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
@@ -1321,16 +1309,16 @@
     </row>
     <row r="22" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="8" t="s">
+      <c r="B22" s="5"/>
+      <c r="C22" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
@@ -1360,13 +1348,13 @@
     <row r="23" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
@@ -1396,13 +1384,13 @@
     <row r="24" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
@@ -1432,13 +1420,13 @@
     <row r="25" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
@@ -1468,13 +1456,13 @@
     <row r="26" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
@@ -1504,13 +1492,13 @@
     <row r="27" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
@@ -1540,13 +1528,13 @@
     <row r="28" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
@@ -1576,13 +1564,13 @@
     <row r="29" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
@@ -1612,13 +1600,13 @@
     <row r="30" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
@@ -1648,13 +1636,13 @@
     <row r="31" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
@@ -1684,13 +1672,13 @@
     <row r="32" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
@@ -1720,13 +1708,13 @@
     <row r="33" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
@@ -1756,13 +1744,13 @@
     <row r="34" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
@@ -1792,13 +1780,13 @@
     <row r="35" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
@@ -1828,13 +1816,13 @@
     <row r="36" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
@@ -1864,13 +1852,13 @@
     <row r="37" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
@@ -1900,13 +1888,13 @@
     <row r="38" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
@@ -1936,13 +1924,13 @@
     <row r="39" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="8"/>
-      <c r="I39" s="8"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
@@ -1972,13 +1960,13 @@
     <row r="40" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
-      <c r="I40" s="8"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6"/>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
@@ -2008,13 +1996,13 @@
     <row r="41" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="8"/>
-      <c r="I41" s="8"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
+      <c r="I41" s="6"/>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
@@ -2044,13 +2032,13 @@
     <row r="42" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="8"/>
-      <c r="H42" s="8"/>
-      <c r="I42" s="8"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="6"/>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
@@ -2080,13 +2068,13 @@
     <row r="43" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="8"/>
-      <c r="E43" s="8"/>
-      <c r="F43" s="8"/>
-      <c r="G43" s="8"/>
-      <c r="H43" s="8"/>
-      <c r="I43" s="8"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="6"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
@@ -2116,13 +2104,13 @@
     <row r="44" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8"/>
-      <c r="F44" s="8"/>
-      <c r="G44" s="8"/>
-      <c r="H44" s="8"/>
-      <c r="I44" s="8"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="6"/>
+      <c r="I44" s="6"/>
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
@@ -2152,13 +2140,13 @@
     <row r="45" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="8"/>
-      <c r="F45" s="8"/>
-      <c r="G45" s="8"/>
-      <c r="H45" s="8"/>
-      <c r="I45" s="8"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
+      <c r="I45" s="6"/>
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
@@ -2188,13 +2176,13 @@
     <row r="46" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="8"/>
-      <c r="E46" s="8"/>
-      <c r="F46" s="8"/>
-      <c r="G46" s="8"/>
-      <c r="H46" s="8"/>
-      <c r="I46" s="8"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
+      <c r="I46" s="6"/>
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
@@ -2224,13 +2212,13 @@
     <row r="47" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="8"/>
-      <c r="E47" s="8"/>
-      <c r="F47" s="8"/>
-      <c r="G47" s="8"/>
-      <c r="H47" s="8"/>
-      <c r="I47" s="8"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="6"/>
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
@@ -2260,13 +2248,13 @@
     <row r="48" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="8"/>
-      <c r="E48" s="8"/>
-      <c r="F48" s="8"/>
-      <c r="G48" s="8"/>
-      <c r="H48" s="8"/>
-      <c r="I48" s="8"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
+      <c r="I48" s="6"/>
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
@@ -2296,13 +2284,13 @@
     <row r="49" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="8"/>
-      <c r="E49" s="8"/>
-      <c r="F49" s="8"/>
-      <c r="G49" s="8"/>
-      <c r="H49" s="8"/>
-      <c r="I49" s="8"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
+      <c r="I49" s="6"/>
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
@@ -2332,13 +2320,13 @@
     <row r="50" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="8"/>
-      <c r="E50" s="8"/>
-      <c r="F50" s="8"/>
-      <c r="G50" s="8"/>
-      <c r="H50" s="8"/>
-      <c r="I50" s="8"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="6"/>
+      <c r="I50" s="6"/>
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
       <c r="L50" s="1"/>
@@ -2368,13 +2356,13 @@
     <row r="51" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="8"/>
-      <c r="F51" s="8"/>
-      <c r="G51" s="8"/>
-      <c r="H51" s="8"/>
-      <c r="I51" s="8"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="6"/>
+      <c r="I51" s="6"/>
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
       <c r="L51" s="1"/>
@@ -2404,13 +2392,13 @@
     <row r="52" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
-      <c r="C52" s="8"/>
-      <c r="D52" s="8"/>
-      <c r="E52" s="8"/>
-      <c r="F52" s="8"/>
-      <c r="G52" s="8"/>
-      <c r="H52" s="8"/>
-      <c r="I52" s="8"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+      <c r="H52" s="6"/>
+      <c r="I52" s="6"/>
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
       <c r="L52" s="1"/>
@@ -2440,13 +2428,13 @@
     <row r="53" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
-      <c r="C53" s="8"/>
-      <c r="D53" s="8"/>
-      <c r="E53" s="8"/>
-      <c r="F53" s="8"/>
-      <c r="G53" s="8"/>
-      <c r="H53" s="8"/>
-      <c r="I53" s="8"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
+      <c r="H53" s="6"/>
+      <c r="I53" s="6"/>
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
       <c r="L53" s="1"/>
@@ -2476,13 +2464,13 @@
     <row r="54" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
-      <c r="C54" s="8"/>
-      <c r="D54" s="8"/>
-      <c r="E54" s="8"/>
-      <c r="F54" s="8"/>
-      <c r="G54" s="8"/>
-      <c r="H54" s="8"/>
-      <c r="I54" s="8"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="6"/>
+      <c r="I54" s="6"/>
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
       <c r="L54" s="1"/>
@@ -2512,13 +2500,13 @@
     <row r="55" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
-      <c r="C55" s="8"/>
-      <c r="D55" s="8"/>
-      <c r="E55" s="8"/>
-      <c r="F55" s="8"/>
-      <c r="G55" s="8"/>
-      <c r="H55" s="8"/>
-      <c r="I55" s="8"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="6"/>
+      <c r="H55" s="6"/>
+      <c r="I55" s="6"/>
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
       <c r="L55" s="1"/>
@@ -2548,13 +2536,13 @@
     <row r="56" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
-      <c r="C56" s="8"/>
-      <c r="D56" s="8"/>
-      <c r="E56" s="8"/>
-      <c r="F56" s="8"/>
-      <c r="G56" s="8"/>
-      <c r="H56" s="8"/>
-      <c r="I56" s="8"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="6"/>
+      <c r="G56" s="6"/>
+      <c r="H56" s="6"/>
+      <c r="I56" s="6"/>
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
       <c r="L56" s="1"/>
@@ -2584,13 +2572,13 @@
     <row r="57" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
-      <c r="C57" s="8"/>
-      <c r="D57" s="8"/>
-      <c r="E57" s="8"/>
-      <c r="F57" s="8"/>
-      <c r="G57" s="8"/>
-      <c r="H57" s="8"/>
-      <c r="I57" s="8"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="6"/>
+      <c r="H57" s="6"/>
+      <c r="I57" s="6"/>
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
       <c r="L57" s="1"/>
@@ -2620,13 +2608,13 @@
     <row r="58" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
-      <c r="C58" s="8"/>
-      <c r="D58" s="8"/>
-      <c r="E58" s="8"/>
-      <c r="F58" s="8"/>
-      <c r="G58" s="8"/>
-      <c r="H58" s="8"/>
-      <c r="I58" s="8"/>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="6"/>
+      <c r="F58" s="6"/>
+      <c r="G58" s="6"/>
+      <c r="H58" s="6"/>
+      <c r="I58" s="6"/>
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
       <c r="L58" s="1"/>
@@ -2656,13 +2644,13 @@
     <row r="59" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
-      <c r="C59" s="8"/>
-      <c r="D59" s="8"/>
-      <c r="E59" s="8"/>
-      <c r="F59" s="8"/>
-      <c r="G59" s="8"/>
-      <c r="H59" s="8"/>
-      <c r="I59" s="8"/>
+      <c r="C59" s="6"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="6"/>
+      <c r="G59" s="6"/>
+      <c r="H59" s="6"/>
+      <c r="I59" s="6"/>
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
       <c r="L59" s="1"/>
@@ -2692,13 +2680,13 @@
     <row r="60" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
-      <c r="C60" s="8"/>
-      <c r="D60" s="8"/>
-      <c r="E60" s="8"/>
-      <c r="F60" s="8"/>
-      <c r="G60" s="8"/>
-      <c r="H60" s="8"/>
-      <c r="I60" s="8"/>
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="6"/>
+      <c r="G60" s="6"/>
+      <c r="H60" s="6"/>
+      <c r="I60" s="6"/>
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
       <c r="L60" s="1"/>
@@ -2728,13 +2716,13 @@
     <row r="61" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
-      <c r="C61" s="8"/>
-      <c r="D61" s="8"/>
-      <c r="E61" s="8"/>
-      <c r="F61" s="8"/>
-      <c r="G61" s="8"/>
-      <c r="H61" s="8"/>
-      <c r="I61" s="8"/>
+      <c r="C61" s="6"/>
+      <c r="D61" s="6"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="6"/>
+      <c r="G61" s="6"/>
+      <c r="H61" s="6"/>
+      <c r="I61" s="6"/>
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
       <c r="L61" s="1"/>
@@ -2764,13 +2752,13 @@
     <row r="62" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
-      <c r="C62" s="8"/>
-      <c r="D62" s="8"/>
-      <c r="E62" s="8"/>
-      <c r="F62" s="8"/>
-      <c r="G62" s="8"/>
-      <c r="H62" s="8"/>
-      <c r="I62" s="8"/>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="6"/>
+      <c r="F62" s="6"/>
+      <c r="G62" s="6"/>
+      <c r="H62" s="6"/>
+      <c r="I62" s="6"/>
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
       <c r="L62" s="1"/>
@@ -2800,13 +2788,13 @@
     <row r="63" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
-      <c r="C63" s="8"/>
-      <c r="D63" s="8"/>
-      <c r="E63" s="8"/>
-      <c r="F63" s="8"/>
-      <c r="G63" s="8"/>
-      <c r="H63" s="8"/>
-      <c r="I63" s="8"/>
+      <c r="C63" s="6"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="6"/>
+      <c r="H63" s="6"/>
+      <c r="I63" s="6"/>
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
       <c r="L63" s="1"/>
@@ -2836,13 +2824,13 @@
     <row r="64" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
-      <c r="C64" s="8"/>
-      <c r="D64" s="8"/>
-      <c r="E64" s="8"/>
-      <c r="F64" s="8"/>
-      <c r="G64" s="8"/>
-      <c r="H64" s="8"/>
-      <c r="I64" s="8"/>
+      <c r="C64" s="6"/>
+      <c r="D64" s="6"/>
+      <c r="E64" s="6"/>
+      <c r="F64" s="6"/>
+      <c r="G64" s="6"/>
+      <c r="H64" s="6"/>
+      <c r="I64" s="6"/>
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
       <c r="L64" s="1"/>
@@ -2872,13 +2860,13 @@
     <row r="65" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
-      <c r="C65" s="8"/>
-      <c r="D65" s="8"/>
-      <c r="E65" s="8"/>
-      <c r="F65" s="8"/>
-      <c r="G65" s="8"/>
-      <c r="H65" s="8"/>
-      <c r="I65" s="8"/>
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="6"/>
+      <c r="F65" s="6"/>
+      <c r="G65" s="6"/>
+      <c r="H65" s="6"/>
+      <c r="I65" s="6"/>
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
       <c r="L65" s="1"/>
@@ -2908,13 +2896,13 @@
     <row r="66" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
-      <c r="C66" s="8"/>
-      <c r="D66" s="8"/>
-      <c r="E66" s="8"/>
-      <c r="F66" s="8"/>
-      <c r="G66" s="8"/>
-      <c r="H66" s="8"/>
-      <c r="I66" s="8"/>
+      <c r="C66" s="6"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="6"/>
+      <c r="F66" s="6"/>
+      <c r="G66" s="6"/>
+      <c r="H66" s="6"/>
+      <c r="I66" s="6"/>
       <c r="J66" s="1"/>
       <c r="K66" s="1"/>
       <c r="L66" s="1"/>
@@ -2944,13 +2932,13 @@
     <row r="67" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
-      <c r="C67" s="8"/>
-      <c r="D67" s="8"/>
-      <c r="E67" s="8"/>
-      <c r="F67" s="8"/>
-      <c r="G67" s="8"/>
-      <c r="H67" s="8"/>
-      <c r="I67" s="8"/>
+      <c r="C67" s="6"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="6"/>
+      <c r="G67" s="6"/>
+      <c r="H67" s="6"/>
+      <c r="I67" s="6"/>
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>
@@ -2980,13 +2968,13 @@
     <row r="68" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
-      <c r="C68" s="8"/>
-      <c r="D68" s="8"/>
-      <c r="E68" s="8"/>
-      <c r="F68" s="8"/>
-      <c r="G68" s="8"/>
-      <c r="H68" s="8"/>
-      <c r="I68" s="8"/>
+      <c r="C68" s="6"/>
+      <c r="D68" s="6"/>
+      <c r="E68" s="6"/>
+      <c r="F68" s="6"/>
+      <c r="G68" s="6"/>
+      <c r="H68" s="6"/>
+      <c r="I68" s="6"/>
       <c r="J68" s="1"/>
       <c r="K68" s="1"/>
       <c r="L68" s="1"/>
@@ -3016,13 +3004,13 @@
     <row r="69" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
-      <c r="C69" s="8"/>
-      <c r="D69" s="8"/>
-      <c r="E69" s="8"/>
-      <c r="F69" s="8"/>
-      <c r="G69" s="8"/>
-      <c r="H69" s="8"/>
-      <c r="I69" s="8"/>
+      <c r="C69" s="6"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="6"/>
+      <c r="G69" s="6"/>
+      <c r="H69" s="6"/>
+      <c r="I69" s="6"/>
       <c r="J69" s="1"/>
       <c r="K69" s="1"/>
       <c r="L69" s="1"/>
@@ -3052,13 +3040,13 @@
     <row r="70" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
-      <c r="C70" s="8"/>
-      <c r="D70" s="8"/>
-      <c r="E70" s="8"/>
-      <c r="F70" s="8"/>
-      <c r="G70" s="8"/>
-      <c r="H70" s="8"/>
-      <c r="I70" s="8"/>
+      <c r="C70" s="6"/>
+      <c r="D70" s="6"/>
+      <c r="E70" s="6"/>
+      <c r="F70" s="6"/>
+      <c r="G70" s="6"/>
+      <c r="H70" s="6"/>
+      <c r="I70" s="6"/>
       <c r="J70" s="1"/>
       <c r="K70" s="1"/>
       <c r="L70" s="1"/>
@@ -3088,13 +3076,13 @@
     <row r="71" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
-      <c r="C71" s="8"/>
-      <c r="D71" s="8"/>
-      <c r="E71" s="8"/>
-      <c r="F71" s="8"/>
-      <c r="G71" s="8"/>
-      <c r="H71" s="8"/>
-      <c r="I71" s="8"/>
+      <c r="C71" s="6"/>
+      <c r="D71" s="6"/>
+      <c r="E71" s="6"/>
+      <c r="F71" s="6"/>
+      <c r="G71" s="6"/>
+      <c r="H71" s="6"/>
+      <c r="I71" s="6"/>
       <c r="J71" s="1"/>
       <c r="K71" s="1"/>
       <c r="L71" s="1"/>
@@ -3124,13 +3112,13 @@
     <row r="72" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
-      <c r="C72" s="8"/>
-      <c r="D72" s="8"/>
-      <c r="E72" s="8"/>
-      <c r="F72" s="8"/>
-      <c r="G72" s="8"/>
-      <c r="H72" s="8"/>
-      <c r="I72" s="8"/>
+      <c r="C72" s="6"/>
+      <c r="D72" s="6"/>
+      <c r="E72" s="6"/>
+      <c r="F72" s="6"/>
+      <c r="G72" s="6"/>
+      <c r="H72" s="6"/>
+      <c r="I72" s="6"/>
       <c r="J72" s="1"/>
       <c r="K72" s="1"/>
       <c r="L72" s="1"/>
@@ -3160,13 +3148,13 @@
     <row r="73" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
-      <c r="C73" s="8"/>
-      <c r="D73" s="8"/>
-      <c r="E73" s="8"/>
-      <c r="F73" s="8"/>
-      <c r="G73" s="8"/>
-      <c r="H73" s="8"/>
-      <c r="I73" s="8"/>
+      <c r="C73" s="6"/>
+      <c r="D73" s="6"/>
+      <c r="E73" s="6"/>
+      <c r="F73" s="6"/>
+      <c r="G73" s="6"/>
+      <c r="H73" s="6"/>
+      <c r="I73" s="6"/>
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
       <c r="L73" s="1"/>
@@ -3196,13 +3184,13 @@
     <row r="74" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
-      <c r="C74" s="8"/>
-      <c r="D74" s="8"/>
-      <c r="E74" s="8"/>
-      <c r="F74" s="8"/>
-      <c r="G74" s="8"/>
-      <c r="H74" s="8"/>
-      <c r="I74" s="8"/>
+      <c r="C74" s="6"/>
+      <c r="D74" s="6"/>
+      <c r="E74" s="6"/>
+      <c r="F74" s="6"/>
+      <c r="G74" s="6"/>
+      <c r="H74" s="6"/>
+      <c r="I74" s="6"/>
       <c r="J74" s="1"/>
       <c r="K74" s="1"/>
       <c r="L74" s="1"/>
@@ -3232,13 +3220,13 @@
     <row r="75" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
-      <c r="C75" s="8"/>
-      <c r="D75" s="8"/>
-      <c r="E75" s="8"/>
-      <c r="F75" s="8"/>
-      <c r="G75" s="8"/>
-      <c r="H75" s="8"/>
-      <c r="I75" s="8"/>
+      <c r="C75" s="6"/>
+      <c r="D75" s="6"/>
+      <c r="E75" s="6"/>
+      <c r="F75" s="6"/>
+      <c r="G75" s="6"/>
+      <c r="H75" s="6"/>
+      <c r="I75" s="6"/>
       <c r="J75" s="1"/>
       <c r="K75" s="1"/>
       <c r="L75" s="1"/>
@@ -6444,60 +6432,11 @@
     </row>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="C56:I56"/>
-    <mergeCell ref="C57:I57"/>
-    <mergeCell ref="C58:I58"/>
-    <mergeCell ref="C59:I59"/>
-    <mergeCell ref="C60:I60"/>
-    <mergeCell ref="C61:I61"/>
-    <mergeCell ref="C62:I62"/>
-    <mergeCell ref="C63:I63"/>
-    <mergeCell ref="C64:I64"/>
-    <mergeCell ref="C65:I65"/>
-    <mergeCell ref="C74:I74"/>
-    <mergeCell ref="C75:I75"/>
-    <mergeCell ref="C66:I66"/>
-    <mergeCell ref="C67:I67"/>
-    <mergeCell ref="C68:I68"/>
-    <mergeCell ref="C69:I69"/>
-    <mergeCell ref="C70:I70"/>
-    <mergeCell ref="C71:I71"/>
-    <mergeCell ref="C72:I72"/>
-    <mergeCell ref="C73:I73"/>
-    <mergeCell ref="C54:I54"/>
-    <mergeCell ref="C55:I55"/>
-    <mergeCell ref="C46:I46"/>
-    <mergeCell ref="C47:I47"/>
-    <mergeCell ref="C48:I48"/>
-    <mergeCell ref="C49:I49"/>
-    <mergeCell ref="C50:I50"/>
-    <mergeCell ref="C51:I51"/>
-    <mergeCell ref="C53:I53"/>
-    <mergeCell ref="C42:I42"/>
-    <mergeCell ref="C43:I43"/>
-    <mergeCell ref="C44:I44"/>
-    <mergeCell ref="C45:I45"/>
-    <mergeCell ref="C52:I52"/>
-    <mergeCell ref="C37:I37"/>
-    <mergeCell ref="C38:I38"/>
-    <mergeCell ref="C39:I39"/>
-    <mergeCell ref="C40:I40"/>
-    <mergeCell ref="C41:I41"/>
-    <mergeCell ref="C32:I32"/>
-    <mergeCell ref="C33:I33"/>
-    <mergeCell ref="C34:I34"/>
-    <mergeCell ref="C35:I35"/>
-    <mergeCell ref="C36:I36"/>
-    <mergeCell ref="C27:I27"/>
-    <mergeCell ref="C28:I28"/>
-    <mergeCell ref="C29:I29"/>
-    <mergeCell ref="C30:I30"/>
-    <mergeCell ref="C31:I31"/>
-    <mergeCell ref="C22:I22"/>
-    <mergeCell ref="C23:I23"/>
-    <mergeCell ref="C24:I24"/>
-    <mergeCell ref="C25:I25"/>
-    <mergeCell ref="C26:I26"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="C3:I3"/>
+    <mergeCell ref="C4:I4"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="C7:I7"/>
     <mergeCell ref="C19:I19"/>
     <mergeCell ref="C20:I20"/>
     <mergeCell ref="C21:I21"/>
@@ -6513,11 +6452,60 @@
     <mergeCell ref="C15:I15"/>
     <mergeCell ref="C16:I16"/>
     <mergeCell ref="B18:I18"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="C3:I3"/>
-    <mergeCell ref="C4:I4"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="C7:I7"/>
+    <mergeCell ref="C22:I22"/>
+    <mergeCell ref="C23:I23"/>
+    <mergeCell ref="C24:I24"/>
+    <mergeCell ref="C25:I25"/>
+    <mergeCell ref="C26:I26"/>
+    <mergeCell ref="C27:I27"/>
+    <mergeCell ref="C28:I28"/>
+    <mergeCell ref="C29:I29"/>
+    <mergeCell ref="C30:I30"/>
+    <mergeCell ref="C31:I31"/>
+    <mergeCell ref="C32:I32"/>
+    <mergeCell ref="C33:I33"/>
+    <mergeCell ref="C34:I34"/>
+    <mergeCell ref="C35:I35"/>
+    <mergeCell ref="C36:I36"/>
+    <mergeCell ref="C37:I37"/>
+    <mergeCell ref="C38:I38"/>
+    <mergeCell ref="C39:I39"/>
+    <mergeCell ref="C40:I40"/>
+    <mergeCell ref="C41:I41"/>
+    <mergeCell ref="C42:I42"/>
+    <mergeCell ref="C43:I43"/>
+    <mergeCell ref="C44:I44"/>
+    <mergeCell ref="C45:I45"/>
+    <mergeCell ref="C52:I52"/>
+    <mergeCell ref="C54:I54"/>
+    <mergeCell ref="C55:I55"/>
+    <mergeCell ref="C46:I46"/>
+    <mergeCell ref="C47:I47"/>
+    <mergeCell ref="C48:I48"/>
+    <mergeCell ref="C49:I49"/>
+    <mergeCell ref="C50:I50"/>
+    <mergeCell ref="C51:I51"/>
+    <mergeCell ref="C53:I53"/>
+    <mergeCell ref="C74:I74"/>
+    <mergeCell ref="C75:I75"/>
+    <mergeCell ref="C66:I66"/>
+    <mergeCell ref="C67:I67"/>
+    <mergeCell ref="C68:I68"/>
+    <mergeCell ref="C69:I69"/>
+    <mergeCell ref="C70:I70"/>
+    <mergeCell ref="C71:I71"/>
+    <mergeCell ref="C72:I72"/>
+    <mergeCell ref="C73:I73"/>
+    <mergeCell ref="C61:I61"/>
+    <mergeCell ref="C62:I62"/>
+    <mergeCell ref="C63:I63"/>
+    <mergeCell ref="C64:I64"/>
+    <mergeCell ref="C65:I65"/>
+    <mergeCell ref="C56:I56"/>
+    <mergeCell ref="C57:I57"/>
+    <mergeCell ref="C58:I58"/>
+    <mergeCell ref="C59:I59"/>
+    <mergeCell ref="C60:I60"/>
   </mergeCells>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6525,6 +6513,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101001CF815299FD08446828E528E2628D888" ma:contentTypeVersion="18" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="eda16f0b0df14eff352f61fdd29391dd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f2ea13ae-bb87-41e3-80ee-445ef9952b1b" xmlns:ns4="7e6392ed-20ae-4cf8-a2eb-b9a38b6c7442" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="39a5156d44086f184d4900c1f32878c2" ns3:_="" ns4:_="">
     <xsd:import namespace="f2ea13ae-bb87-41e3-80ee-445ef9952b1b"/>
@@ -6777,15 +6774,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -6795,6 +6783,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{511756B6-1F99-4910-A3C6-88D26ECE21F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{544664A2-1060-4B74-93C6-D9FAA1CADC8A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6809,14 +6805,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{511756B6-1F99-4910-A3C6-88D26ECE21F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
pequeña comprobacion e implementacion de perfil
</commit_message>
<xml_diff>
--- a/por hacer.xlsx
+++ b/por hacer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proyecto mayo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F00CC3-3FE1-4F7E-9A83-10500266034B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2067B98-ED54-4ADF-BFDB-7AD9BFBEED46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2736" yWindow="1440" windowWidth="18948" windowHeight="10656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -503,7 +503,7 @@
   <dimension ref="A1:AH164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1309,7 +1309,7 @@
     </row>
     <row r="22" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
-      <c r="B22" s="5"/>
+      <c r="B22" s="3"/>
       <c r="C22" s="6" t="s">
         <v>18</v>
       </c>
@@ -6432,11 +6432,60 @@
     </row>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="C3:I3"/>
-    <mergeCell ref="C4:I4"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="C7:I7"/>
+    <mergeCell ref="C56:I56"/>
+    <mergeCell ref="C57:I57"/>
+    <mergeCell ref="C58:I58"/>
+    <mergeCell ref="C59:I59"/>
+    <mergeCell ref="C60:I60"/>
+    <mergeCell ref="C61:I61"/>
+    <mergeCell ref="C62:I62"/>
+    <mergeCell ref="C63:I63"/>
+    <mergeCell ref="C64:I64"/>
+    <mergeCell ref="C65:I65"/>
+    <mergeCell ref="C74:I74"/>
+    <mergeCell ref="C75:I75"/>
+    <mergeCell ref="C66:I66"/>
+    <mergeCell ref="C67:I67"/>
+    <mergeCell ref="C68:I68"/>
+    <mergeCell ref="C69:I69"/>
+    <mergeCell ref="C70:I70"/>
+    <mergeCell ref="C71:I71"/>
+    <mergeCell ref="C72:I72"/>
+    <mergeCell ref="C73:I73"/>
+    <mergeCell ref="C54:I54"/>
+    <mergeCell ref="C55:I55"/>
+    <mergeCell ref="C46:I46"/>
+    <mergeCell ref="C47:I47"/>
+    <mergeCell ref="C48:I48"/>
+    <mergeCell ref="C49:I49"/>
+    <mergeCell ref="C50:I50"/>
+    <mergeCell ref="C51:I51"/>
+    <mergeCell ref="C53:I53"/>
+    <mergeCell ref="C42:I42"/>
+    <mergeCell ref="C43:I43"/>
+    <mergeCell ref="C44:I44"/>
+    <mergeCell ref="C45:I45"/>
+    <mergeCell ref="C52:I52"/>
+    <mergeCell ref="C37:I37"/>
+    <mergeCell ref="C38:I38"/>
+    <mergeCell ref="C39:I39"/>
+    <mergeCell ref="C40:I40"/>
+    <mergeCell ref="C41:I41"/>
+    <mergeCell ref="C32:I32"/>
+    <mergeCell ref="C33:I33"/>
+    <mergeCell ref="C34:I34"/>
+    <mergeCell ref="C35:I35"/>
+    <mergeCell ref="C36:I36"/>
+    <mergeCell ref="C27:I27"/>
+    <mergeCell ref="C28:I28"/>
+    <mergeCell ref="C29:I29"/>
+    <mergeCell ref="C30:I30"/>
+    <mergeCell ref="C31:I31"/>
+    <mergeCell ref="C22:I22"/>
+    <mergeCell ref="C23:I23"/>
+    <mergeCell ref="C24:I24"/>
+    <mergeCell ref="C25:I25"/>
+    <mergeCell ref="C26:I26"/>
     <mergeCell ref="C19:I19"/>
     <mergeCell ref="C20:I20"/>
     <mergeCell ref="C21:I21"/>
@@ -6452,60 +6501,11 @@
     <mergeCell ref="C15:I15"/>
     <mergeCell ref="C16:I16"/>
     <mergeCell ref="B18:I18"/>
-    <mergeCell ref="C22:I22"/>
-    <mergeCell ref="C23:I23"/>
-    <mergeCell ref="C24:I24"/>
-    <mergeCell ref="C25:I25"/>
-    <mergeCell ref="C26:I26"/>
-    <mergeCell ref="C27:I27"/>
-    <mergeCell ref="C28:I28"/>
-    <mergeCell ref="C29:I29"/>
-    <mergeCell ref="C30:I30"/>
-    <mergeCell ref="C31:I31"/>
-    <mergeCell ref="C32:I32"/>
-    <mergeCell ref="C33:I33"/>
-    <mergeCell ref="C34:I34"/>
-    <mergeCell ref="C35:I35"/>
-    <mergeCell ref="C36:I36"/>
-    <mergeCell ref="C37:I37"/>
-    <mergeCell ref="C38:I38"/>
-    <mergeCell ref="C39:I39"/>
-    <mergeCell ref="C40:I40"/>
-    <mergeCell ref="C41:I41"/>
-    <mergeCell ref="C42:I42"/>
-    <mergeCell ref="C43:I43"/>
-    <mergeCell ref="C44:I44"/>
-    <mergeCell ref="C45:I45"/>
-    <mergeCell ref="C52:I52"/>
-    <mergeCell ref="C54:I54"/>
-    <mergeCell ref="C55:I55"/>
-    <mergeCell ref="C46:I46"/>
-    <mergeCell ref="C47:I47"/>
-    <mergeCell ref="C48:I48"/>
-    <mergeCell ref="C49:I49"/>
-    <mergeCell ref="C50:I50"/>
-    <mergeCell ref="C51:I51"/>
-    <mergeCell ref="C53:I53"/>
-    <mergeCell ref="C74:I74"/>
-    <mergeCell ref="C75:I75"/>
-    <mergeCell ref="C66:I66"/>
-    <mergeCell ref="C67:I67"/>
-    <mergeCell ref="C68:I68"/>
-    <mergeCell ref="C69:I69"/>
-    <mergeCell ref="C70:I70"/>
-    <mergeCell ref="C71:I71"/>
-    <mergeCell ref="C72:I72"/>
-    <mergeCell ref="C73:I73"/>
-    <mergeCell ref="C61:I61"/>
-    <mergeCell ref="C62:I62"/>
-    <mergeCell ref="C63:I63"/>
-    <mergeCell ref="C64:I64"/>
-    <mergeCell ref="C65:I65"/>
-    <mergeCell ref="C56:I56"/>
-    <mergeCell ref="C57:I57"/>
-    <mergeCell ref="C58:I58"/>
-    <mergeCell ref="C59:I59"/>
-    <mergeCell ref="C60:I60"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="C3:I3"/>
+    <mergeCell ref="C4:I4"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="C7:I7"/>
   </mergeCells>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6513,15 +6513,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101001CF815299FD08446828E528E2628D888" ma:contentTypeVersion="18" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="eda16f0b0df14eff352f61fdd29391dd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f2ea13ae-bb87-41e3-80ee-445ef9952b1b" xmlns:ns4="7e6392ed-20ae-4cf8-a2eb-b9a38b6c7442" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="39a5156d44086f184d4900c1f32878c2" ns3:_="" ns4:_="">
     <xsd:import namespace="f2ea13ae-bb87-41e3-80ee-445ef9952b1b"/>
@@ -6774,6 +6765,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -6783,14 +6783,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{511756B6-1F99-4910-A3C6-88D26ECE21F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{544664A2-1060-4B74-93C6-D9FAA1CADC8A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6805,6 +6797,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{511756B6-1F99-4910-A3C6-88D26ECE21F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Creacion del logo y ajuste en las contraseñas de los formularios
</commit_message>
<xml_diff>
--- a/por hacer.xlsx
+++ b/por hacer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proyecto mayo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2067B98-ED54-4ADF-BFDB-7AD9BFBEED46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69398128-7318-444C-B074-C16571676869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2736" yWindow="1440" windowWidth="18948" windowHeight="10656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -503,7 +503,7 @@
   <dimension ref="A1:AH164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -587,7 +587,7 @@
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="B3" s="5"/>
+      <c r="B3" s="3"/>
       <c r="C3" s="6" t="s">
         <v>0</v>
       </c>
@@ -1081,7 +1081,7 @@
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
-      <c r="B16" s="5"/>
+      <c r="B16" s="3"/>
       <c r="C16" s="6" t="s">
         <v>15</v>
       </c>
@@ -6432,60 +6432,11 @@
     </row>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="C56:I56"/>
-    <mergeCell ref="C57:I57"/>
-    <mergeCell ref="C58:I58"/>
-    <mergeCell ref="C59:I59"/>
-    <mergeCell ref="C60:I60"/>
-    <mergeCell ref="C61:I61"/>
-    <mergeCell ref="C62:I62"/>
-    <mergeCell ref="C63:I63"/>
-    <mergeCell ref="C64:I64"/>
-    <mergeCell ref="C65:I65"/>
-    <mergeCell ref="C74:I74"/>
-    <mergeCell ref="C75:I75"/>
-    <mergeCell ref="C66:I66"/>
-    <mergeCell ref="C67:I67"/>
-    <mergeCell ref="C68:I68"/>
-    <mergeCell ref="C69:I69"/>
-    <mergeCell ref="C70:I70"/>
-    <mergeCell ref="C71:I71"/>
-    <mergeCell ref="C72:I72"/>
-    <mergeCell ref="C73:I73"/>
-    <mergeCell ref="C54:I54"/>
-    <mergeCell ref="C55:I55"/>
-    <mergeCell ref="C46:I46"/>
-    <mergeCell ref="C47:I47"/>
-    <mergeCell ref="C48:I48"/>
-    <mergeCell ref="C49:I49"/>
-    <mergeCell ref="C50:I50"/>
-    <mergeCell ref="C51:I51"/>
-    <mergeCell ref="C53:I53"/>
-    <mergeCell ref="C42:I42"/>
-    <mergeCell ref="C43:I43"/>
-    <mergeCell ref="C44:I44"/>
-    <mergeCell ref="C45:I45"/>
-    <mergeCell ref="C52:I52"/>
-    <mergeCell ref="C37:I37"/>
-    <mergeCell ref="C38:I38"/>
-    <mergeCell ref="C39:I39"/>
-    <mergeCell ref="C40:I40"/>
-    <mergeCell ref="C41:I41"/>
-    <mergeCell ref="C32:I32"/>
-    <mergeCell ref="C33:I33"/>
-    <mergeCell ref="C34:I34"/>
-    <mergeCell ref="C35:I35"/>
-    <mergeCell ref="C36:I36"/>
-    <mergeCell ref="C27:I27"/>
-    <mergeCell ref="C28:I28"/>
-    <mergeCell ref="C29:I29"/>
-    <mergeCell ref="C30:I30"/>
-    <mergeCell ref="C31:I31"/>
-    <mergeCell ref="C22:I22"/>
-    <mergeCell ref="C23:I23"/>
-    <mergeCell ref="C24:I24"/>
-    <mergeCell ref="C25:I25"/>
-    <mergeCell ref="C26:I26"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="C3:I3"/>
+    <mergeCell ref="C4:I4"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="C7:I7"/>
     <mergeCell ref="C19:I19"/>
     <mergeCell ref="C20:I20"/>
     <mergeCell ref="C21:I21"/>
@@ -6501,11 +6452,60 @@
     <mergeCell ref="C15:I15"/>
     <mergeCell ref="C16:I16"/>
     <mergeCell ref="B18:I18"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="C3:I3"/>
-    <mergeCell ref="C4:I4"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="C7:I7"/>
+    <mergeCell ref="C22:I22"/>
+    <mergeCell ref="C23:I23"/>
+    <mergeCell ref="C24:I24"/>
+    <mergeCell ref="C25:I25"/>
+    <mergeCell ref="C26:I26"/>
+    <mergeCell ref="C27:I27"/>
+    <mergeCell ref="C28:I28"/>
+    <mergeCell ref="C29:I29"/>
+    <mergeCell ref="C30:I30"/>
+    <mergeCell ref="C31:I31"/>
+    <mergeCell ref="C32:I32"/>
+    <mergeCell ref="C33:I33"/>
+    <mergeCell ref="C34:I34"/>
+    <mergeCell ref="C35:I35"/>
+    <mergeCell ref="C36:I36"/>
+    <mergeCell ref="C37:I37"/>
+    <mergeCell ref="C38:I38"/>
+    <mergeCell ref="C39:I39"/>
+    <mergeCell ref="C40:I40"/>
+    <mergeCell ref="C41:I41"/>
+    <mergeCell ref="C42:I42"/>
+    <mergeCell ref="C43:I43"/>
+    <mergeCell ref="C44:I44"/>
+    <mergeCell ref="C45:I45"/>
+    <mergeCell ref="C52:I52"/>
+    <mergeCell ref="C54:I54"/>
+    <mergeCell ref="C55:I55"/>
+    <mergeCell ref="C46:I46"/>
+    <mergeCell ref="C47:I47"/>
+    <mergeCell ref="C48:I48"/>
+    <mergeCell ref="C49:I49"/>
+    <mergeCell ref="C50:I50"/>
+    <mergeCell ref="C51:I51"/>
+    <mergeCell ref="C53:I53"/>
+    <mergeCell ref="C74:I74"/>
+    <mergeCell ref="C75:I75"/>
+    <mergeCell ref="C66:I66"/>
+    <mergeCell ref="C67:I67"/>
+    <mergeCell ref="C68:I68"/>
+    <mergeCell ref="C69:I69"/>
+    <mergeCell ref="C70:I70"/>
+    <mergeCell ref="C71:I71"/>
+    <mergeCell ref="C72:I72"/>
+    <mergeCell ref="C73:I73"/>
+    <mergeCell ref="C61:I61"/>
+    <mergeCell ref="C62:I62"/>
+    <mergeCell ref="C63:I63"/>
+    <mergeCell ref="C64:I64"/>
+    <mergeCell ref="C65:I65"/>
+    <mergeCell ref="C56:I56"/>
+    <mergeCell ref="C57:I57"/>
+    <mergeCell ref="C58:I58"/>
+    <mergeCell ref="C59:I59"/>
+    <mergeCell ref="C60:I60"/>
   </mergeCells>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6513,6 +6513,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101001CF815299FD08446828E528E2628D888" ma:contentTypeVersion="18" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="eda16f0b0df14eff352f61fdd29391dd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f2ea13ae-bb87-41e3-80ee-445ef9952b1b" xmlns:ns4="7e6392ed-20ae-4cf8-a2eb-b9a38b6c7442" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="39a5156d44086f184d4900c1f32878c2" ns3:_="" ns4:_="">
     <xsd:import namespace="f2ea13ae-bb87-41e3-80ee-445ef9952b1b"/>
@@ -6765,15 +6774,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -6783,6 +6783,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{511756B6-1F99-4910-A3C6-88D26ECE21F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{544664A2-1060-4B74-93C6-D9FAA1CADC8A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6797,14 +6805,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{511756B6-1F99-4910-A3C6-88D26ECE21F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
comprobacion extra para mal inicio
</commit_message>
<xml_diff>
--- a/por hacer.xlsx
+++ b/por hacer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proyecto mayo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69398128-7318-444C-B074-C16571676869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D321B3-FBF3-48D0-8474-0372F85E94DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2736" yWindow="1440" windowWidth="18948" windowHeight="10656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -111,7 +111,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -121,12 +121,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -143,7 +137,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -155,9 +149,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -503,7 +494,7 @@
   <dimension ref="A1:AH164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -549,16 +540,16 @@
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -588,15 +579,15 @@
     <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="3"/>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -625,16 +616,16 @@
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="6" t="s">
+      <c r="B4" s="3"/>
+      <c r="C4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
@@ -663,16 +654,16 @@
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="6" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -701,16 +692,16 @@
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -740,15 +731,15 @@
     <row r="7" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="4"/>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -778,15 +769,15 @@
     <row r="8" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="4"/>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
@@ -816,15 +807,15 @@
     <row r="9" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="4"/>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
@@ -854,15 +845,15 @@
     <row r="10" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="4"/>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
@@ -892,15 +883,15 @@
     <row r="11" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="4"/>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
@@ -929,16 +920,16 @@
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
@@ -968,15 +959,15 @@
     <row r="13" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="3"/>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
@@ -1006,15 +997,15 @@
     <row r="14" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="3"/>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
       <c r="J14" s="2"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
@@ -1044,15 +1035,15 @@
     <row r="15" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="3"/>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -1082,15 +1073,15 @@
     <row r="16" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="3"/>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -1120,15 +1111,15 @@
     <row r="17" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="3"/>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
@@ -1157,16 +1148,16 @@
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
@@ -1196,15 +1187,15 @@
     <row r="19" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="3"/>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
@@ -1234,15 +1225,15 @@
     <row r="20" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="3"/>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
@@ -1272,15 +1263,15 @@
     <row r="21" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="3"/>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
@@ -1310,15 +1301,15 @@
     <row r="22" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="3"/>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
@@ -1348,13 +1339,13 @@
     <row r="23" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
@@ -1384,13 +1375,13 @@
     <row r="24" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
@@ -1420,13 +1411,13 @@
     <row r="25" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
@@ -1456,13 +1447,13 @@
     <row r="26" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
@@ -1492,13 +1483,13 @@
     <row r="27" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
@@ -1528,13 +1519,13 @@
     <row r="28" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
@@ -1564,13 +1555,13 @@
     <row r="29" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
@@ -1600,13 +1591,13 @@
     <row r="30" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
@@ -1636,13 +1627,13 @@
     <row r="31" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
@@ -1672,13 +1663,13 @@
     <row r="32" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
@@ -1708,13 +1699,13 @@
     <row r="33" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
@@ -1744,13 +1735,13 @@
     <row r="34" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
@@ -1780,13 +1771,13 @@
     <row r="35" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="6"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
@@ -1816,13 +1807,13 @@
     <row r="36" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
@@ -1852,13 +1843,13 @@
     <row r="37" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
@@ -1888,13 +1879,13 @@
     <row r="38" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="6"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
@@ -1924,13 +1915,13 @@
     <row r="39" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
-      <c r="I39" s="6"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
@@ -1960,13 +1951,13 @@
     <row r="40" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
-      <c r="H40" s="6"/>
-      <c r="I40" s="6"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
@@ -1996,13 +1987,13 @@
     <row r="41" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
-      <c r="H41" s="6"/>
-      <c r="I41" s="6"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
@@ -2032,13 +2023,13 @@
     <row r="42" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
-      <c r="H42" s="6"/>
-      <c r="I42" s="6"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="5"/>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
@@ -2068,13 +2059,13 @@
     <row r="43" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
-      <c r="F43" s="6"/>
-      <c r="G43" s="6"/>
-      <c r="H43" s="6"/>
-      <c r="I43" s="6"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
@@ -2104,13 +2095,13 @@
     <row r="44" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="6"/>
-      <c r="G44" s="6"/>
-      <c r="H44" s="6"/>
-      <c r="I44" s="6"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
@@ -2140,13 +2131,13 @@
     <row r="45" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
-      <c r="G45" s="6"/>
-      <c r="H45" s="6"/>
-      <c r="I45" s="6"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
@@ -2176,13 +2167,13 @@
     <row r="46" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="6"/>
-      <c r="G46" s="6"/>
-      <c r="H46" s="6"/>
-      <c r="I46" s="6"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
+      <c r="I46" s="5"/>
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
@@ -2212,13 +2203,13 @@
     <row r="47" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="6"/>
-      <c r="G47" s="6"/>
-      <c r="H47" s="6"/>
-      <c r="I47" s="6"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="5"/>
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
@@ -2248,13 +2239,13 @@
     <row r="48" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
-      <c r="F48" s="6"/>
-      <c r="G48" s="6"/>
-      <c r="H48" s="6"/>
-      <c r="I48" s="6"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
+      <c r="I48" s="5"/>
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
@@ -2284,13 +2275,13 @@
     <row r="49" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
-      <c r="C49" s="6"/>
-      <c r="D49" s="6"/>
-      <c r="E49" s="6"/>
-      <c r="F49" s="6"/>
-      <c r="G49" s="6"/>
-      <c r="H49" s="6"/>
-      <c r="I49" s="6"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5"/>
+      <c r="I49" s="5"/>
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
@@ -2320,13 +2311,13 @@
     <row r="50" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
-      <c r="F50" s="6"/>
-      <c r="G50" s="6"/>
-      <c r="H50" s="6"/>
-      <c r="I50" s="6"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="5"/>
+      <c r="I50" s="5"/>
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
       <c r="L50" s="1"/>
@@ -2356,13 +2347,13 @@
     <row r="51" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
-      <c r="C51" s="6"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="6"/>
-      <c r="G51" s="6"/>
-      <c r="H51" s="6"/>
-      <c r="I51" s="6"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
+      <c r="H51" s="5"/>
+      <c r="I51" s="5"/>
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
       <c r="L51" s="1"/>
@@ -2392,13 +2383,13 @@
     <row r="52" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
-      <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="6"/>
-      <c r="F52" s="6"/>
-      <c r="G52" s="6"/>
-      <c r="H52" s="6"/>
-      <c r="I52" s="6"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="5"/>
+      <c r="I52" s="5"/>
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
       <c r="L52" s="1"/>
@@ -2428,13 +2419,13 @@
     <row r="53" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="6"/>
-      <c r="E53" s="6"/>
-      <c r="F53" s="6"/>
-      <c r="G53" s="6"/>
-      <c r="H53" s="6"/>
-      <c r="I53" s="6"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="5"/>
+      <c r="I53" s="5"/>
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
       <c r="L53" s="1"/>
@@ -2464,13 +2455,13 @@
     <row r="54" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
-      <c r="C54" s="6"/>
-      <c r="D54" s="6"/>
-      <c r="E54" s="6"/>
-      <c r="F54" s="6"/>
-      <c r="G54" s="6"/>
-      <c r="H54" s="6"/>
-      <c r="I54" s="6"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="5"/>
+      <c r="I54" s="5"/>
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
       <c r="L54" s="1"/>
@@ -2500,13 +2491,13 @@
     <row r="55" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
-      <c r="C55" s="6"/>
-      <c r="D55" s="6"/>
-      <c r="E55" s="6"/>
-      <c r="F55" s="6"/>
-      <c r="G55" s="6"/>
-      <c r="H55" s="6"/>
-      <c r="I55" s="6"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
+      <c r="G55" s="5"/>
+      <c r="H55" s="5"/>
+      <c r="I55" s="5"/>
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
       <c r="L55" s="1"/>
@@ -2536,13 +2527,13 @@
     <row r="56" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
-      <c r="C56" s="6"/>
-      <c r="D56" s="6"/>
-      <c r="E56" s="6"/>
-      <c r="F56" s="6"/>
-      <c r="G56" s="6"/>
-      <c r="H56" s="6"/>
-      <c r="I56" s="6"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="5"/>
+      <c r="I56" s="5"/>
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
       <c r="L56" s="1"/>
@@ -2572,13 +2563,13 @@
     <row r="57" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
-      <c r="C57" s="6"/>
-      <c r="D57" s="6"/>
-      <c r="E57" s="6"/>
-      <c r="F57" s="6"/>
-      <c r="G57" s="6"/>
-      <c r="H57" s="6"/>
-      <c r="I57" s="6"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
+      <c r="G57" s="5"/>
+      <c r="H57" s="5"/>
+      <c r="I57" s="5"/>
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
       <c r="L57" s="1"/>
@@ -2608,13 +2599,13 @@
     <row r="58" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
-      <c r="C58" s="6"/>
-      <c r="D58" s="6"/>
-      <c r="E58" s="6"/>
-      <c r="F58" s="6"/>
-      <c r="G58" s="6"/>
-      <c r="H58" s="6"/>
-      <c r="I58" s="6"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="5"/>
+      <c r="G58" s="5"/>
+      <c r="H58" s="5"/>
+      <c r="I58" s="5"/>
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
       <c r="L58" s="1"/>
@@ -2644,13 +2635,13 @@
     <row r="59" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
-      <c r="C59" s="6"/>
-      <c r="D59" s="6"/>
-      <c r="E59" s="6"/>
-      <c r="F59" s="6"/>
-      <c r="G59" s="6"/>
-      <c r="H59" s="6"/>
-      <c r="I59" s="6"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="5"/>
+      <c r="F59" s="5"/>
+      <c r="G59" s="5"/>
+      <c r="H59" s="5"/>
+      <c r="I59" s="5"/>
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
       <c r="L59" s="1"/>
@@ -2680,13 +2671,13 @@
     <row r="60" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
-      <c r="C60" s="6"/>
-      <c r="D60" s="6"/>
-      <c r="E60" s="6"/>
-      <c r="F60" s="6"/>
-      <c r="G60" s="6"/>
-      <c r="H60" s="6"/>
-      <c r="I60" s="6"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="5"/>
+      <c r="F60" s="5"/>
+      <c r="G60" s="5"/>
+      <c r="H60" s="5"/>
+      <c r="I60" s="5"/>
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
       <c r="L60" s="1"/>
@@ -2716,13 +2707,13 @@
     <row r="61" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
-      <c r="C61" s="6"/>
-      <c r="D61" s="6"/>
-      <c r="E61" s="6"/>
-      <c r="F61" s="6"/>
-      <c r="G61" s="6"/>
-      <c r="H61" s="6"/>
-      <c r="I61" s="6"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
+      <c r="E61" s="5"/>
+      <c r="F61" s="5"/>
+      <c r="G61" s="5"/>
+      <c r="H61" s="5"/>
+      <c r="I61" s="5"/>
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
       <c r="L61" s="1"/>
@@ -2752,13 +2743,13 @@
     <row r="62" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
-      <c r="C62" s="6"/>
-      <c r="D62" s="6"/>
-      <c r="E62" s="6"/>
-      <c r="F62" s="6"/>
-      <c r="G62" s="6"/>
-      <c r="H62" s="6"/>
-      <c r="I62" s="6"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
+      <c r="E62" s="5"/>
+      <c r="F62" s="5"/>
+      <c r="G62" s="5"/>
+      <c r="H62" s="5"/>
+      <c r="I62" s="5"/>
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
       <c r="L62" s="1"/>
@@ -2788,13 +2779,13 @@
     <row r="63" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
-      <c r="C63" s="6"/>
-      <c r="D63" s="6"/>
-      <c r="E63" s="6"/>
-      <c r="F63" s="6"/>
-      <c r="G63" s="6"/>
-      <c r="H63" s="6"/>
-      <c r="I63" s="6"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="5"/>
+      <c r="F63" s="5"/>
+      <c r="G63" s="5"/>
+      <c r="H63" s="5"/>
+      <c r="I63" s="5"/>
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
       <c r="L63" s="1"/>
@@ -2824,13 +2815,13 @@
     <row r="64" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
-      <c r="C64" s="6"/>
-      <c r="D64" s="6"/>
-      <c r="E64" s="6"/>
-      <c r="F64" s="6"/>
-      <c r="G64" s="6"/>
-      <c r="H64" s="6"/>
-      <c r="I64" s="6"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
+      <c r="E64" s="5"/>
+      <c r="F64" s="5"/>
+      <c r="G64" s="5"/>
+      <c r="H64" s="5"/>
+      <c r="I64" s="5"/>
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
       <c r="L64" s="1"/>
@@ -2860,13 +2851,13 @@
     <row r="65" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
-      <c r="C65" s="6"/>
-      <c r="D65" s="6"/>
-      <c r="E65" s="6"/>
-      <c r="F65" s="6"/>
-      <c r="G65" s="6"/>
-      <c r="H65" s="6"/>
-      <c r="I65" s="6"/>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
+      <c r="E65" s="5"/>
+      <c r="F65" s="5"/>
+      <c r="G65" s="5"/>
+      <c r="H65" s="5"/>
+      <c r="I65" s="5"/>
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
       <c r="L65" s="1"/>
@@ -2896,13 +2887,13 @@
     <row r="66" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
-      <c r="C66" s="6"/>
-      <c r="D66" s="6"/>
-      <c r="E66" s="6"/>
-      <c r="F66" s="6"/>
-      <c r="G66" s="6"/>
-      <c r="H66" s="6"/>
-      <c r="I66" s="6"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="5"/>
+      <c r="E66" s="5"/>
+      <c r="F66" s="5"/>
+      <c r="G66" s="5"/>
+      <c r="H66" s="5"/>
+      <c r="I66" s="5"/>
       <c r="J66" s="1"/>
       <c r="K66" s="1"/>
       <c r="L66" s="1"/>
@@ -2932,13 +2923,13 @@
     <row r="67" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
-      <c r="C67" s="6"/>
-      <c r="D67" s="6"/>
-      <c r="E67" s="6"/>
-      <c r="F67" s="6"/>
-      <c r="G67" s="6"/>
-      <c r="H67" s="6"/>
-      <c r="I67" s="6"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
+      <c r="E67" s="5"/>
+      <c r="F67" s="5"/>
+      <c r="G67" s="5"/>
+      <c r="H67" s="5"/>
+      <c r="I67" s="5"/>
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>
@@ -2968,13 +2959,13 @@
     <row r="68" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
-      <c r="C68" s="6"/>
-      <c r="D68" s="6"/>
-      <c r="E68" s="6"/>
-      <c r="F68" s="6"/>
-      <c r="G68" s="6"/>
-      <c r="H68" s="6"/>
-      <c r="I68" s="6"/>
+      <c r="C68" s="5"/>
+      <c r="D68" s="5"/>
+      <c r="E68" s="5"/>
+      <c r="F68" s="5"/>
+      <c r="G68" s="5"/>
+      <c r="H68" s="5"/>
+      <c r="I68" s="5"/>
       <c r="J68" s="1"/>
       <c r="K68" s="1"/>
       <c r="L68" s="1"/>
@@ -3004,13 +2995,13 @@
     <row r="69" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
-      <c r="C69" s="6"/>
-      <c r="D69" s="6"/>
-      <c r="E69" s="6"/>
-      <c r="F69" s="6"/>
-      <c r="G69" s="6"/>
-      <c r="H69" s="6"/>
-      <c r="I69" s="6"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
+      <c r="E69" s="5"/>
+      <c r="F69" s="5"/>
+      <c r="G69" s="5"/>
+      <c r="H69" s="5"/>
+      <c r="I69" s="5"/>
       <c r="J69" s="1"/>
       <c r="K69" s="1"/>
       <c r="L69" s="1"/>
@@ -3040,13 +3031,13 @@
     <row r="70" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
-      <c r="C70" s="6"/>
-      <c r="D70" s="6"/>
-      <c r="E70" s="6"/>
-      <c r="F70" s="6"/>
-      <c r="G70" s="6"/>
-      <c r="H70" s="6"/>
-      <c r="I70" s="6"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
+      <c r="E70" s="5"/>
+      <c r="F70" s="5"/>
+      <c r="G70" s="5"/>
+      <c r="H70" s="5"/>
+      <c r="I70" s="5"/>
       <c r="J70" s="1"/>
       <c r="K70" s="1"/>
       <c r="L70" s="1"/>
@@ -3076,13 +3067,13 @@
     <row r="71" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
-      <c r="C71" s="6"/>
-      <c r="D71" s="6"/>
-      <c r="E71" s="6"/>
-      <c r="F71" s="6"/>
-      <c r="G71" s="6"/>
-      <c r="H71" s="6"/>
-      <c r="I71" s="6"/>
+      <c r="C71" s="5"/>
+      <c r="D71" s="5"/>
+      <c r="E71" s="5"/>
+      <c r="F71" s="5"/>
+      <c r="G71" s="5"/>
+      <c r="H71" s="5"/>
+      <c r="I71" s="5"/>
       <c r="J71" s="1"/>
       <c r="K71" s="1"/>
       <c r="L71" s="1"/>
@@ -3112,13 +3103,13 @@
     <row r="72" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
-      <c r="C72" s="6"/>
-      <c r="D72" s="6"/>
-      <c r="E72" s="6"/>
-      <c r="F72" s="6"/>
-      <c r="G72" s="6"/>
-      <c r="H72" s="6"/>
-      <c r="I72" s="6"/>
+      <c r="C72" s="5"/>
+      <c r="D72" s="5"/>
+      <c r="E72" s="5"/>
+      <c r="F72" s="5"/>
+      <c r="G72" s="5"/>
+      <c r="H72" s="5"/>
+      <c r="I72" s="5"/>
       <c r="J72" s="1"/>
       <c r="K72" s="1"/>
       <c r="L72" s="1"/>
@@ -3148,13 +3139,13 @@
     <row r="73" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
-      <c r="C73" s="6"/>
-      <c r="D73" s="6"/>
-      <c r="E73" s="6"/>
-      <c r="F73" s="6"/>
-      <c r="G73" s="6"/>
-      <c r="H73" s="6"/>
-      <c r="I73" s="6"/>
+      <c r="C73" s="5"/>
+      <c r="D73" s="5"/>
+      <c r="E73" s="5"/>
+      <c r="F73" s="5"/>
+      <c r="G73" s="5"/>
+      <c r="H73" s="5"/>
+      <c r="I73" s="5"/>
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
       <c r="L73" s="1"/>
@@ -3184,13 +3175,13 @@
     <row r="74" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
-      <c r="C74" s="6"/>
-      <c r="D74" s="6"/>
-      <c r="E74" s="6"/>
-      <c r="F74" s="6"/>
-      <c r="G74" s="6"/>
-      <c r="H74" s="6"/>
-      <c r="I74" s="6"/>
+      <c r="C74" s="5"/>
+      <c r="D74" s="5"/>
+      <c r="E74" s="5"/>
+      <c r="F74" s="5"/>
+      <c r="G74" s="5"/>
+      <c r="H74" s="5"/>
+      <c r="I74" s="5"/>
       <c r="J74" s="1"/>
       <c r="K74" s="1"/>
       <c r="L74" s="1"/>
@@ -3220,13 +3211,13 @@
     <row r="75" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
-      <c r="C75" s="6"/>
-      <c r="D75" s="6"/>
-      <c r="E75" s="6"/>
-      <c r="F75" s="6"/>
-      <c r="G75" s="6"/>
-      <c r="H75" s="6"/>
-      <c r="I75" s="6"/>
+      <c r="C75" s="5"/>
+      <c r="D75" s="5"/>
+      <c r="E75" s="5"/>
+      <c r="F75" s="5"/>
+      <c r="G75" s="5"/>
+      <c r="H75" s="5"/>
+      <c r="I75" s="5"/>
       <c r="J75" s="1"/>
       <c r="K75" s="1"/>
       <c r="L75" s="1"/>
@@ -6432,11 +6423,60 @@
     </row>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="C3:I3"/>
-    <mergeCell ref="C4:I4"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="C7:I7"/>
+    <mergeCell ref="C56:I56"/>
+    <mergeCell ref="C57:I57"/>
+    <mergeCell ref="C58:I58"/>
+    <mergeCell ref="C59:I59"/>
+    <mergeCell ref="C60:I60"/>
+    <mergeCell ref="C61:I61"/>
+    <mergeCell ref="C62:I62"/>
+    <mergeCell ref="C63:I63"/>
+    <mergeCell ref="C64:I64"/>
+    <mergeCell ref="C65:I65"/>
+    <mergeCell ref="C74:I74"/>
+    <mergeCell ref="C75:I75"/>
+    <mergeCell ref="C66:I66"/>
+    <mergeCell ref="C67:I67"/>
+    <mergeCell ref="C68:I68"/>
+    <mergeCell ref="C69:I69"/>
+    <mergeCell ref="C70:I70"/>
+    <mergeCell ref="C71:I71"/>
+    <mergeCell ref="C72:I72"/>
+    <mergeCell ref="C73:I73"/>
+    <mergeCell ref="C54:I54"/>
+    <mergeCell ref="C55:I55"/>
+    <mergeCell ref="C46:I46"/>
+    <mergeCell ref="C47:I47"/>
+    <mergeCell ref="C48:I48"/>
+    <mergeCell ref="C49:I49"/>
+    <mergeCell ref="C50:I50"/>
+    <mergeCell ref="C51:I51"/>
+    <mergeCell ref="C53:I53"/>
+    <mergeCell ref="C42:I42"/>
+    <mergeCell ref="C43:I43"/>
+    <mergeCell ref="C44:I44"/>
+    <mergeCell ref="C45:I45"/>
+    <mergeCell ref="C52:I52"/>
+    <mergeCell ref="C37:I37"/>
+    <mergeCell ref="C38:I38"/>
+    <mergeCell ref="C39:I39"/>
+    <mergeCell ref="C40:I40"/>
+    <mergeCell ref="C41:I41"/>
+    <mergeCell ref="C32:I32"/>
+    <mergeCell ref="C33:I33"/>
+    <mergeCell ref="C34:I34"/>
+    <mergeCell ref="C35:I35"/>
+    <mergeCell ref="C36:I36"/>
+    <mergeCell ref="C27:I27"/>
+    <mergeCell ref="C28:I28"/>
+    <mergeCell ref="C29:I29"/>
+    <mergeCell ref="C30:I30"/>
+    <mergeCell ref="C31:I31"/>
+    <mergeCell ref="C22:I22"/>
+    <mergeCell ref="C23:I23"/>
+    <mergeCell ref="C24:I24"/>
+    <mergeCell ref="C25:I25"/>
+    <mergeCell ref="C26:I26"/>
     <mergeCell ref="C19:I19"/>
     <mergeCell ref="C20:I20"/>
     <mergeCell ref="C21:I21"/>
@@ -6452,60 +6492,11 @@
     <mergeCell ref="C15:I15"/>
     <mergeCell ref="C16:I16"/>
     <mergeCell ref="B18:I18"/>
-    <mergeCell ref="C22:I22"/>
-    <mergeCell ref="C23:I23"/>
-    <mergeCell ref="C24:I24"/>
-    <mergeCell ref="C25:I25"/>
-    <mergeCell ref="C26:I26"/>
-    <mergeCell ref="C27:I27"/>
-    <mergeCell ref="C28:I28"/>
-    <mergeCell ref="C29:I29"/>
-    <mergeCell ref="C30:I30"/>
-    <mergeCell ref="C31:I31"/>
-    <mergeCell ref="C32:I32"/>
-    <mergeCell ref="C33:I33"/>
-    <mergeCell ref="C34:I34"/>
-    <mergeCell ref="C35:I35"/>
-    <mergeCell ref="C36:I36"/>
-    <mergeCell ref="C37:I37"/>
-    <mergeCell ref="C38:I38"/>
-    <mergeCell ref="C39:I39"/>
-    <mergeCell ref="C40:I40"/>
-    <mergeCell ref="C41:I41"/>
-    <mergeCell ref="C42:I42"/>
-    <mergeCell ref="C43:I43"/>
-    <mergeCell ref="C44:I44"/>
-    <mergeCell ref="C45:I45"/>
-    <mergeCell ref="C52:I52"/>
-    <mergeCell ref="C54:I54"/>
-    <mergeCell ref="C55:I55"/>
-    <mergeCell ref="C46:I46"/>
-    <mergeCell ref="C47:I47"/>
-    <mergeCell ref="C48:I48"/>
-    <mergeCell ref="C49:I49"/>
-    <mergeCell ref="C50:I50"/>
-    <mergeCell ref="C51:I51"/>
-    <mergeCell ref="C53:I53"/>
-    <mergeCell ref="C74:I74"/>
-    <mergeCell ref="C75:I75"/>
-    <mergeCell ref="C66:I66"/>
-    <mergeCell ref="C67:I67"/>
-    <mergeCell ref="C68:I68"/>
-    <mergeCell ref="C69:I69"/>
-    <mergeCell ref="C70:I70"/>
-    <mergeCell ref="C71:I71"/>
-    <mergeCell ref="C72:I72"/>
-    <mergeCell ref="C73:I73"/>
-    <mergeCell ref="C61:I61"/>
-    <mergeCell ref="C62:I62"/>
-    <mergeCell ref="C63:I63"/>
-    <mergeCell ref="C64:I64"/>
-    <mergeCell ref="C65:I65"/>
-    <mergeCell ref="C56:I56"/>
-    <mergeCell ref="C57:I57"/>
-    <mergeCell ref="C58:I58"/>
-    <mergeCell ref="C59:I59"/>
-    <mergeCell ref="C60:I60"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="C3:I3"/>
+    <mergeCell ref="C4:I4"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="C7:I7"/>
   </mergeCells>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6513,15 +6504,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101001CF815299FD08446828E528E2628D888" ma:contentTypeVersion="18" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="eda16f0b0df14eff352f61fdd29391dd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f2ea13ae-bb87-41e3-80ee-445ef9952b1b" xmlns:ns4="7e6392ed-20ae-4cf8-a2eb-b9a38b6c7442" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="39a5156d44086f184d4900c1f32878c2" ns3:_="" ns4:_="">
     <xsd:import namespace="f2ea13ae-bb87-41e3-80ee-445ef9952b1b"/>
@@ -6774,6 +6756,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -6783,14 +6774,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{511756B6-1F99-4910-A3C6-88D26ECE21F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{544664A2-1060-4B74-93C6-D9FAA1CADC8A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6805,6 +6788,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{511756B6-1F99-4910-A3C6-88D26ECE21F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>